<commit_message>
satellites get destroyed when touching Earth
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>Status</t>
   </si>
@@ -162,9 +162,6 @@
     <t xml:space="preserve">creat game object from prefab</t>
   </si>
   <si>
-    <t xml:space="preserve">adjust graphics of new sat</t>
-  </si>
-  <si>
     <t xml:space="preserve">add sat to list</t>
   </si>
   <si>
@@ -222,25 +219,28 @@
     <t xml:space="preserve">data relay</t>
   </si>
   <si>
-    <t>on/off</t>
+    <t>passive</t>
   </si>
   <si>
     <t>imagery</t>
   </si>
   <si>
-    <t xml:space="preserve">image area</t>
+    <t xml:space="preserve">show area to image</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
   <si>
     <t>experiment</t>
   </si>
   <si>
-    <t xml:space="preserve">when to run</t>
+    <t>run</t>
   </si>
   <si>
     <t xml:space="preserve">grapple arm</t>
   </si>
   <si>
-    <t>go-ahead</t>
+    <t>attach/detach</t>
   </si>
   <si>
     <t>maneuver</t>
@@ -279,19 +279,13 @@
     <t xml:space="preserve">fuel level, battery, etc.</t>
   </si>
   <si>
-    <t>integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bug fixes</t>
-  </si>
-  <si>
     <t xml:space="preserve">satellite motion</t>
   </si>
   <si>
     <t xml:space="preserve">sat de-orbit mechanics</t>
   </si>
   <si>
-    <t xml:space="preserve">burn-up at x km</t>
+    <t xml:space="preserve">burn-up at 100 km</t>
   </si>
   <si>
     <t xml:space="preserve">atmospheric drag</t>
@@ -549,7 +543,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -579,9 +573,6 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -589,6 +580,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -614,7 +611,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J123" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J119" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1124,7 +1121,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A62" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1179,13 +1176,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.22950819672131148</v>
+        <v>0.23728813559322035</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I121,"0")/ROWS(Table5[])</f>
-        <v>1.6393442622950821e-002</v>
+        <f>COUNTIF(I2:I117,"0")/ROWS(Table5[])</f>
+        <v>2.5423728813559324e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1222,7 +1219,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1656,7 +1653,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>38</v>
@@ -1765,23 +1762,25 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="6"/>
+      <c r="I40" s="6">
+        <v>1</v>
+      </c>
       <c r="J40" s="9"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="C41" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="11" t="s">
-        <v>50</v>
-      </c>
+      <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -1791,25 +1790,26 @@
     <row r="42" ht="14.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="4"/>
+      <c r="D42" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="6"/>
+      <c r="I42" s="6">
+        <v>1</v>
+      </c>
       <c r="J42" s="9"/>
     </row>
     <row r="43" ht="28.5">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
@@ -1822,63 +1822,64 @@
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="6">
+      <c r="I44" s="12">
         <v>1</v>
       </c>
       <c r="J44" s="9"/>
     </row>
     <row r="45" ht="28.5">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4" t="s">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
       <c r="I45" s="13">
         <v>1</v>
       </c>
-      <c r="J45" s="9"/>
+      <c r="J45" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" ht="28.5">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="14">
-        <v>1</v>
-      </c>
-      <c r="J46" s="10" t="s">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="9"/>
     </row>
     <row r="47" ht="28.5">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
-      <c r="I47" s="6"/>
+      <c r="I47" s="6">
+        <v>1</v>
+      </c>
       <c r="J47" s="9"/>
     </row>
     <row r="48" ht="28.5">
@@ -1886,16 +1887,18 @@
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="6">
         <v>1</v>
       </c>
-      <c r="J48" s="9"/>
+      <c r="J48" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="49" ht="28.5">
       <c r="A49" s="4"/>
@@ -1904,7 +1907,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -1912,7 +1915,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" ht="28.5">
@@ -1922,7 +1925,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -1930,58 +1933,56 @@
         <v>1</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" ht="28.5">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="6">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="13">
         <v>1</v>
       </c>
-      <c r="J51" s="9" t="s">
-        <v>64</v>
+      <c r="J51" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="52" ht="28.5">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="14">
-        <v>1</v>
-      </c>
-      <c r="J52" s="10" t="s">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="9"/>
     </row>
     <row r="53" ht="28.5">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="4"/>
+      <c r="F53" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="6"/>
-      <c r="J53" s="9"/>
+      <c r="J53" s="14" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="54" ht="14.25">
       <c r="A54" s="4"/>
@@ -1990,12 +1991,12 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="6"/>
-      <c r="J54" s="9"/>
+      <c r="J54" s="14"/>
     </row>
     <row r="55" ht="14.25">
       <c r="A55" s="4"/>
@@ -2004,8 +2005,8 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="12" t="s">
-        <v>69</v>
+      <c r="G55" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="6"/>
@@ -2017,10 +2018,10 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="15" t="s">
+        <v>71</v>
+      </c>
       <c r="H56" s="4"/>
       <c r="I56" s="6"/>
       <c r="J56" s="9"/>
@@ -2031,13 +2032,15 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="F57" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="6"/>
-      <c r="J57" s="9"/>
+      <c r="J57" s="14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="58" ht="14.25">
       <c r="A58" s="4"/>
@@ -2046,25 +2049,29 @@
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="6"/>
-      <c r="J58" s="9"/>
+      <c r="J58" s="14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="59" ht="14.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="F59" s="4"/>
-      <c r="G59" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="G59" s="4"/>
       <c r="H59" s="4"/>
-      <c r="I59" s="6"/>
+      <c r="I59" s="6">
+        <v>1</v>
+      </c>
       <c r="J59" s="9"/>
     </row>
     <row r="60" ht="28.5">
@@ -2074,12 +2081,16 @@
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="9"/>
+      <c r="I60" s="6">
+        <v>1</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="61" ht="28.5">
       <c r="A61" s="4"/>
@@ -2087,46 +2098,52 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="F61" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G61" s="4"/>
       <c r="H61" s="4"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="9"/>
+      <c r="I61" s="6">
+        <v>1</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="62" ht="28.5">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="6">
         <v>1</v>
       </c>
-      <c r="J62" s="9"/>
+      <c r="J62" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="63" ht="28.5">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E63" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="6">
         <v>1</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" ht="28.5">
@@ -2134,17 +2151,17 @@
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="E64" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="6">
         <v>1</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" ht="14.25">
@@ -2152,99 +2169,87 @@
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="E65" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="6">
-        <v>1</v>
-      </c>
+      <c r="I65" s="6"/>
       <c r="J65" s="9" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="D66" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="6">
+      <c r="I66" s="16">
         <v>1</v>
       </c>
-      <c r="J66" s="9" t="s">
-        <v>83</v>
-      </c>
+      <c r="J66" s="9"/>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="D67" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="6">
-        <v>1</v>
-      </c>
-      <c r="J67" s="9" t="s">
-        <v>85</v>
-      </c>
+      <c r="I67" s="6"/>
+      <c r="J67" s="9"/>
     </row>
     <row r="68" ht="14.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-      <c r="E68" s="4" t="s">
-        <v>86</v>
+      <c r="E68" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="6"/>
-      <c r="J68" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="J68" s="9"/>
     </row>
     <row r="69" ht="14.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
-      <c r="D69" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="6"/>
-      <c r="J69" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="J69" s="9"/>
     </row>
     <row r="70" ht="14.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="C70" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="15">
+      <c r="I70" s="6">
         <v>1</v>
       </c>
       <c r="J70" s="9"/>
@@ -2253,38 +2258,44 @@
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="11" t="s">
-        <v>91</v>
+      <c r="D71" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="9"/>
+      <c r="I71" s="6">
+        <v>1</v>
+      </c>
+      <c r="J71" s="9" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11" t="s">
-        <v>92</v>
-      </c>
+      <c r="D72" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="6"/>
-      <c r="J72" s="9"/>
+      <c r="J72" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="C73" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
@@ -2294,73 +2305,67 @@
     <row r="74" ht="14.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
-      <c r="C74" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
-      <c r="I74" s="6">
-        <v>1</v>
-      </c>
+      <c r="I74" s="6"/>
       <c r="J74" s="9"/>
     </row>
     <row r="75" ht="14.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
-      <c r="I75" s="6">
-        <v>1</v>
-      </c>
-      <c r="J75" s="9" t="s">
-        <v>96</v>
-      </c>
+      <c r="I75" s="6"/>
+      <c r="J75" s="9"/>
     </row>
     <row r="76" ht="14.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="9" t="s">
-        <v>98</v>
-      </c>
+      <c r="J76" s="9"/>
     </row>
     <row r="77" ht="14.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="9"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="78" ht="14.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -2375,7 +2380,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -2389,7 +2394,7 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -2398,27 +2403,25 @@
       <c r="J80" s="9"/>
     </row>
     <row r="81" ht="14.25">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="9"/>
     </row>
     <row r="82" ht="14.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -2458,11 +2461,11 @@
     <row r="85" ht="14.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
+      <c r="C85" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="D85" s="4"/>
-      <c r="E85" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -2474,7 +2477,7 @@
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -2487,10 +2490,10 @@
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4" t="s">
-        <v>107</v>
-      </c>
+      <c r="D87" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
@@ -2503,7 +2506,7 @@
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
@@ -2514,12 +2517,12 @@
     <row r="89" ht="14.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
-      <c r="C89" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
+      <c r="F89" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="6"/>
@@ -2529,11 +2532,11 @@
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
-      <c r="D90" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="D90" s="4"/>
       <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
+      <c r="F90" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="6"/>
@@ -2544,7 +2547,7 @@
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
@@ -2559,7 +2562,7 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
@@ -2574,7 +2577,7 @@
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2586,10 +2589,10 @@
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="E94" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="6"/>
@@ -2599,11 +2602,11 @@
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
-      <c r="D95" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="D95" s="4"/>
       <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
+      <c r="F95" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="6"/>
@@ -2615,7 +2618,7 @@
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
@@ -2630,7 +2633,7 @@
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
@@ -2642,8 +2645,8 @@
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="4" t="s">
-        <v>117</v>
+      <c r="E98" s="11" t="s">
+        <v>118</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
@@ -2658,7 +2661,7 @@
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
@@ -2666,41 +2669,41 @@
       <c r="J99" s="9"/>
     </row>
     <row r="100" ht="14.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-      <c r="I100" s="6"/>
-      <c r="J100" s="9"/>
+      <c r="A100" s="11"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="10"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="6"/>
-      <c r="J101" s="9"/>
+      <c r="A101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G101" s="11"/>
+      <c r="H101" s="11"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="10"/>
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-      <c r="E102" s="12" t="s">
+      <c r="D102" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="E102" s="4"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
@@ -2711,53 +2714,53 @@
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
+      <c r="D103" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E103" s="4"/>
-      <c r="F103" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="6"/>
       <c r="J103" s="9"/>
     </row>
     <row r="104" ht="14.25">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
-      <c r="C104" s="12"/>
-      <c r="D104" s="12"/>
-      <c r="E104" s="12" t="s">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F104" s="12"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="12"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="10"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="9"/>
     </row>
     <row r="105" ht="14.25">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
-      <c r="C105" s="12"/>
-      <c r="D105" s="12"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="G105" s="12"/>
-      <c r="H105" s="12"/>
-      <c r="I105" s="14"/>
-      <c r="J105" s="10"/>
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="9"/>
     </row>
     <row r="106" ht="14.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
-      <c r="D106" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="D106" s="4"/>
       <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
+      <c r="F106" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="6"/>
@@ -2767,15 +2770,17 @@
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
-      <c r="D107" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="6"/>
-      <c r="J107" s="9"/>
+      <c r="J107" s="9" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="4"/>
@@ -2783,26 +2788,30 @@
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="6"/>
-      <c r="J108" s="9"/>
+      <c r="J108" s="9" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
+      <c r="D109" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="E109" s="4"/>
-      <c r="F109" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
-      <c r="I109" s="6"/>
+      <c r="I109" s="6">
+        <v>1</v>
+      </c>
       <c r="J109" s="9"/>
     </row>
     <row r="110" ht="14.25">
@@ -2810,13 +2819,15 @@
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4" t="s">
-        <v>125</v>
-      </c>
+      <c r="E110" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
-      <c r="I110" s="6"/>
+      <c r="I110" s="6">
+        <v>1</v>
+      </c>
       <c r="J110" s="9"/>
     </row>
     <row r="111" ht="14.25">
@@ -2825,78 +2836,70 @@
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="6"/>
-      <c r="J111" s="9" t="s">
-        <v>127</v>
-      </c>
+      <c r="I111" s="6">
+        <v>1</v>
+      </c>
+      <c r="J111" s="9"/>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4" t="s">
-        <v>128</v>
-      </c>
+      <c r="D112" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E112" s="4"/>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="6"/>
-      <c r="J112" s="9" t="s">
-        <v>129</v>
-      </c>
+      <c r="J112" s="9"/>
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4" t="s">
+      <c r="C113" s="4" t="s">
         <v>130</v>
       </c>
+      <c r="D113" s="4"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="6">
-        <v>1</v>
-      </c>
+      <c r="I113" s="6"/>
       <c r="J113" s="9"/>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D114" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
-      <c r="I114" s="6">
-        <v>1</v>
-      </c>
+      <c r="I114" s="6"/>
       <c r="J114" s="9"/>
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
-      <c r="D115" s="4"/>
-      <c r="E115" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="D115" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
-      <c r="I115" s="6">
-        <v>1</v>
-      </c>
+      <c r="I115" s="6"/>
       <c r="J115" s="9"/>
     </row>
     <row r="116" ht="14.25">
@@ -2904,7 +2907,7 @@
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -2916,10 +2919,10 @@
     <row r="117" ht="14.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
-      <c r="C117" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
@@ -2929,11 +2932,11 @@
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
+      <c r="B118" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="C118" s="4"/>
-      <c r="D118" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="D118" s="4"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
@@ -2944,10 +2947,10 @@
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="C119" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D119" s="4"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
@@ -2955,62 +2958,10 @@
       <c r="I119" s="6"/>
       <c r="J119" s="9"/>
     </row>
-    <row r="120" ht="14.25">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="6"/>
-      <c r="J120" s="9"/>
-    </row>
-    <row r="121" ht="14.25">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
-      <c r="I121" s="6"/>
-      <c r="J121" s="9"/>
-    </row>
-    <row r="122" ht="14.25">
-      <c r="A122" s="4"/>
-      <c r="B122" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="4"/>
-      <c r="H122" s="4"/>
-      <c r="I122" s="6"/>
-      <c r="J122" s="9"/>
-    </row>
-    <row r="123" ht="14.25">
-      <c r="A123" s="4"/>
-      <c r="B123" s="4"/>
-      <c r="C123" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4"/>
-      <c r="I123" s="6"/>
-      <c r="J123" s="9"/>
-    </row>
+    <row r="120" ht="14.25"/>
+    <row r="121" ht="14.25"/>
+    <row r="122" ht="14.25"/>
+    <row r="123" ht="14.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
@@ -3029,7 +2980,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004F00DA-0023-49BA-BED6-007C00F70069}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004100DF-0038-45E6-B74E-0037001200EF}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3043,10 +2994,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I107 I108:I121 I48:I51</xm:sqref>
+          <xm:sqref>I3:I103 I104:I117 I47:I50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F9009E-009C-4D0D-8112-005900A400CF}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007B005C-00ED-44A7-A91D-00DF00270087}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3060,10 +3011,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I123</xm:sqref>
+          <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00CE000B-00D8-4ACA-979B-00BE005F0072}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006E00AD-001C-4D1B-8967-000400140048}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3077,10 +3028,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I122</xm:sqref>
+          <xm:sqref>I118</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00500074-0092-4F8A-B66A-002D00290026}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D800BC-00F8-495C-92F8-003800290043}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3097,7 +3048,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007600B2-0056-4947-9BAC-006C009400E6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003C0089-0056-44F8-A022-00E1001700BC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3114,7 +3065,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002A00A3-0005-49E3-8440-00070047004F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006100A8-002F-4972-8139-00B6007900AA}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3131,7 +3082,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C900A6-0055-499F-B038-00CB007E0023}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D200BE-0022-4AC0-A314-00450048003B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3145,10 +3096,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I46</xm:sqref>
+          <xm:sqref>I45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00A70021-004E-49A4-B761-004D008700C7}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005C0008-00EF-43CB-8592-00700064004E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3162,10 +3113,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I73</xm:sqref>
+          <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008800FC-00CD-467E-ADB4-0061004500C6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{009300D5-00FD-42F2-8213-00EB001200F7}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3179,10 +3130,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I72</xm:sqref>
+          <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00280023-0005-4A9B-97E0-00A300B0004D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004C0007-00D6-4687-A1FD-00BF007900FF}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3196,10 +3147,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I71</xm:sqref>
+          <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B40007-00FA-40D1-AFCC-00F2005400AC}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00240095-00A6-4950-8534-00CB00240061}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3216,7 +3167,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004F001E-0004-46D5-B910-00EF00CE00DB}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F8000C-00BF-4F07-98AA-003E008300CD}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3230,10 +3181,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I123</xm:sqref>
+          <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008E005F-0052-4FC5-A575-0083005200F3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{006B000A-0017-40DB-9CCC-001E006A0029}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3247,10 +3198,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I107 I108:I121 I48:I51</xm:sqref>
+          <xm:sqref>I3:I103 I104:I117 I47:I50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00FC00C7-0064-469F-897D-0056002800B0}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{006400C2-00C8-49ED-BC0E-00C40090000B}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3267,7 +3218,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009600D6-0090-40C8-A0DF-0059002A00F6}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{008D007B-008F-43D4-B16E-005D00110040}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3281,10 +3232,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I122</xm:sqref>
+          <xm:sqref>I118</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00500012-007E-4086-A2FE-003D00470049}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D50010-004E-4319-BEE3-006B00ED0049}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3301,7 +3252,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008F0083-00AB-4785-A779-00F900030053}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00EF0071-008B-43BB-B3EF-0042008700D9}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3315,10 +3266,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I46</xm:sqref>
+          <xm:sqref>I45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AD0036-00EA-4956-9AA0-004800F50062}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D00020-00EF-45AC-8419-008B00260058}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3332,10 +3283,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I73</xm:sqref>
+          <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007800BA-00DE-4DEB-81F7-0028004700E8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003500B6-00C7-4952-AD68-00C500780062}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3349,10 +3300,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I72</xm:sqref>
+          <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B300A6-0082-441D-90B4-005C003A00F9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001A005C-0086-4C08-AEE8-00BF000A0049}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3366,10 +3317,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I71</xm:sqref>
+          <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00930011-00A1-4427-8C48-00EC009F00D0}">
+          <x14:cfRule type="dataBar" priority="2" id="{00440052-0041-449B-8F2A-001F00D1008F}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3385,7 +3336,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00430018-005E-4228-80CD-00A0005F004A}">
+          <x14:cfRule type="dataBar" priority="1" id="{00B9006B-0031-4FCD-B2C4-00DE00A4006D}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
fixed fuel units, updated tasks
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Status</t>
   </si>
@@ -219,6 +219,9 @@
     <t xml:space="preserve">task payload</t>
   </si>
   <si>
+    <t xml:space="preserve">payloads should be scripts that are attached</t>
+  </si>
+  <si>
     <t xml:space="preserve">data relay</t>
   </si>
   <si>
@@ -231,7 +234,7 @@
     <t xml:space="preserve">show area to image</t>
   </si>
   <si>
-    <t>image</t>
+    <t xml:space="preserve">take image</t>
   </si>
   <si>
     <t>experiment</t>
@@ -588,14 +591,14 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1127,7 +1130,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A104" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1182,13 +1185,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.25210084033613445</v>
+        <v>0.26050420168067229</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I118,"0")/ROWS(Table5[])</f>
-        <v>2.5210084033613446e-002</v>
+        <v>1.680672268907563e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1260,7 +1263,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1659,7 +1662,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>38</v>
@@ -1986,7 +1989,9 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="6"/>
-      <c r="J53" s="9"/>
+      <c r="J53" s="14" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="54" ht="14.25">
       <c r="A54" s="4"/>
@@ -1995,13 +2000,13 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="6"/>
       <c r="J54" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" ht="14.25">
@@ -2011,7 +2016,7 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
@@ -2026,7 +2031,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="6"/>
@@ -2039,8 +2044,8 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
-        <v>72</v>
+      <c r="G57" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="6"/>
@@ -2053,13 +2058,13 @@
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="6"/>
       <c r="J58" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" ht="14.25">
@@ -2069,13 +2074,13 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="6"/>
       <c r="J59" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" ht="28.5">
@@ -2084,7 +2089,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -2109,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" ht="28.5">
@@ -2119,7 +2124,7 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -2127,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" ht="28.5">
@@ -2137,7 +2142,7 @@
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
@@ -2145,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" ht="28.5">
@@ -2154,7 +2159,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2163,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" ht="14.25">
@@ -2172,7 +2177,7 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -2181,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" ht="14.25">
@@ -2190,14 +2195,14 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="6"/>
       <c r="J66" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" ht="14.25">
@@ -2205,13 +2210,13 @@
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="14">
+      <c r="I67" s="16">
         <v>1</v>
       </c>
       <c r="J67" s="9"/>
@@ -2221,7 +2226,7 @@
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -2235,8 +2240,8 @@
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="15" t="s">
-        <v>91</v>
+      <c r="E69" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -2252,7 +2257,7 @@
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -2266,7 +2271,7 @@
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2283,7 +2288,7 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -2293,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" ht="14.25">
@@ -2301,7 +2306,7 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -2309,14 +2314,14 @@
       <c r="H73" s="4"/>
       <c r="I73" s="6"/>
       <c r="J73" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" ht="14.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -2331,7 +2336,7 @@
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -2360,7 +2365,7 @@
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -2373,7 +2378,7 @@
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
@@ -2381,7 +2386,7 @@
       <c r="H78" s="11"/>
       <c r="I78" s="13"/>
       <c r="J78" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" ht="14.25">
@@ -2389,7 +2394,7 @@
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -2404,7 +2409,7 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -2418,7 +2423,7 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -2460,7 +2465,7 @@
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -2474,7 +2479,7 @@
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
@@ -2486,7 +2491,7 @@
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -2501,7 +2506,7 @@
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -2515,7 +2520,7 @@
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -2530,7 +2535,7 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
@@ -2545,7 +2550,7 @@
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
@@ -2559,7 +2564,7 @@
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
       <c r="F91" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
@@ -2571,7 +2576,7 @@
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -2586,7 +2591,7 @@
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
@@ -2601,7 +2606,7 @@
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -2614,7 +2619,7 @@
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
@@ -2629,7 +2634,7 @@
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
@@ -2642,7 +2647,7 @@
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
@@ -2657,7 +2662,7 @@
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
@@ -2670,7 +2675,7 @@
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
@@ -2685,7 +2690,7 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
@@ -2698,7 +2703,7 @@
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F101" s="11"/>
       <c r="G101" s="11"/>
@@ -2713,7 +2718,7 @@
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
@@ -2725,7 +2730,7 @@
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
@@ -2754,7 +2759,7 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
@@ -2769,7 +2774,7 @@
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
@@ -2783,7 +2788,7 @@
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -2796,14 +2801,14 @@
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="6"/>
       <c r="J108" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" ht="14.25">
@@ -2812,14 +2817,14 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="6"/>
       <c r="J109" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="110" ht="14.25">
@@ -2827,7 +2832,7 @@
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
@@ -2860,7 +2865,7 @@
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
@@ -2888,7 +2893,7 @@
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -2903,7 +2908,7 @@
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
@@ -2917,7 +2922,7 @@
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -2931,7 +2936,7 @@
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
@@ -2957,7 +2962,7 @@
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
@@ -2980,8 +2985,8 @@
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="6"/>
-      <c r="J120" s="16" t="s">
-        <v>136</v>
+      <c r="J120" s="9" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="121" ht="14.25"/>
@@ -3005,7 +3010,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0040004B-0071-4CA6-9764-00E800C4008F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004300E1-00FB-401A-A012-006400850052}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3022,7 +3027,7 @@
           <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00AC00A5-001A-4139-8F8C-00CC0019004B}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00EE0077-0075-4B1B-8F13-0000004800CD}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3039,7 +3044,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C30058-003D-4256-9711-000C00270010}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{002D000E-00A6-4931-A3B7-00D700980000}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3056,7 +3061,7 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007F003B-0066-4EA1-873F-006600D800BB}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{000B0077-0072-49E4-95A9-0030008900B9}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3073,7 +3078,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{001E00B8-0048-49B5-825E-00EA00FC00DB}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003400F7-0043-4A92-87F3-00880071005C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3090,7 +3095,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00A30050-0037-48A1-BA43-007F00C70035}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007A00CA-0084-4EEC-AB85-000E006B005F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3107,7 +3112,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00550015-00AF-4E66-86C1-005C00500041}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0054009D-0026-4976-B1B4-002700D500CF}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3124,7 +3129,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003E002E-00CB-487B-8C2F-0090001300AC}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005A0013-001E-440B-8EB4-00EB00D200C9}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3141,7 +3146,7 @@
           <xm:sqref>I70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00AD0056-00CF-4B4A-B1EC-007B006F00D4}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00CA0041-00E4-4857-8C25-00A600C90001}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3158,7 +3163,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B5005D-009F-4EB0-A8D9-00530029004E}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00060032-00F6-485B-AB85-005800E4003F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3175,7 +3180,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AC00A6-0045-4A81-81D8-00A000E70063}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00140064-0053-46ED-98B6-0035009200DD}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3192,7 +3197,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AC00A7-006E-4301-9452-00BF00B6008E}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001D0049-0001-4035-AC80-00260006004B}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3209,7 +3214,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0015006C-00EE-456C-B4B7-006300850000}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00EE00C7-0087-4231-BF11-004600B6008B}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3226,7 +3231,7 @@
           <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00090014-0038-446F-BAF3-000F00A8001D}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{007A00B8-0073-4531-8A75-006600DC00B5}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3243,7 +3248,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00EF0052-00E7-44AC-98FD-009E005600FD}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0056006A-00D6-445C-9D23-008A00F80073}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3260,7 +3265,7 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F100ED-0038-493A-8150-00BB002B00EC}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003C0020-00C3-4629-9C72-006A004C0086}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3277,7 +3282,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007E0041-008D-4023-9D63-006900A700E9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00890090-00D4-44E7-971C-00F1005F0040}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3294,7 +3299,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C800BC-00EB-4EE4-943B-007D00AD002B}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BE0063-00A5-4736-A7C2-00C1007B0008}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3311,7 +3316,7 @@
           <xm:sqref>I70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00470062-007D-4EF1-A0DC-001F00040097}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000300B8-0056-488C-A767-00AD002F00D9}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3328,7 +3333,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0034004A-000F-4A2F-B8CE-004C00D9004B}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{009F00A1-000D-41B1-AFF3-003D00CD00C3}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3345,7 +3350,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{000F001E-0094-4777-829B-0057003B0017}">
+          <x14:cfRule type="dataBar" priority="2" id="{008100A4-0072-4143-AEB2-002E00ED0069}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3361,7 +3366,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{0019009F-00A1-4719-9C5A-0063009E00FE}">
+          <x14:cfRule type="dataBar" priority="1" id="{00BB003B-0031-4432-86D2-00F000E80081}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Started mission dev, reorganized some files
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
   <si>
     <t>Status</t>
   </si>
@@ -234,6 +234,9 @@
     <t xml:space="preserve">show area to image</t>
   </si>
   <si>
+    <t xml:space="preserve">cone from satellite to target </t>
+  </si>
+  <si>
     <t xml:space="preserve">take image</t>
   </si>
   <si>
@@ -345,7 +348,16 @@
     <t xml:space="preserve">mission system</t>
   </si>
   <si>
-    <t xml:space="preserve">probability to give mission</t>
+    <t xml:space="preserve">timer to give new missions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timer set to random time within range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mission type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chance for each mission type</t>
   </si>
   <si>
     <t xml:space="preserve">continuous missions</t>
@@ -594,10 +606,10 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -620,7 +632,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J120" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J121" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1130,7 +1142,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1185,13 +1197,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.26050420168067229</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I118,"0")/ROWS(Table5[])</f>
-        <v>1.680672268907563e-002</v>
+        <f>COUNTIF(I2:I119,"0")/ROWS(Table5[])</f>
+        <v>8.3333333333333332e-003</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1228,7 +1240,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1263,7 +1275,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1627,9 +1639,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="6">
-        <v>0</v>
-      </c>
+      <c r="I31" s="6"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" ht="14.25">
@@ -1989,7 +1999,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="6"/>
-      <c r="J53" s="14" t="s">
+      <c r="J53" s="9" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2035,7 +2045,9 @@
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="6"/>
-      <c r="J56" s="9"/>
+      <c r="J56" s="14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="57" ht="14.25">
       <c r="A57" s="4"/>
@@ -2044,8 +2056,8 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="15" t="s">
-        <v>73</v>
+      <c r="G57" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="6"/>
@@ -2058,13 +2070,13 @@
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="6"/>
       <c r="J58" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" ht="14.25">
@@ -2074,13 +2086,13 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="6"/>
       <c r="J59" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" ht="28.5">
@@ -2089,7 +2101,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -2114,7 +2126,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" ht="28.5">
@@ -2124,7 +2136,7 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -2132,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" ht="28.5">
@@ -2142,7 +2154,7 @@
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
@@ -2150,7 +2162,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" ht="28.5">
@@ -2159,7 +2171,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2168,7 +2180,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" ht="14.25">
@@ -2177,7 +2189,7 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -2186,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" ht="14.25">
@@ -2195,14 +2207,14 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="6"/>
       <c r="J66" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" ht="14.25">
@@ -2210,13 +2222,13 @@
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="16">
+      <c r="I67" s="15">
         <v>1</v>
       </c>
       <c r="J67" s="9"/>
@@ -2226,7 +2238,7 @@
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -2241,7 +2253,7 @@
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -2257,7 +2269,7 @@
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -2271,7 +2283,7 @@
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2288,7 +2300,7 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -2298,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" ht="14.25">
@@ -2306,7 +2318,7 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -2314,14 +2326,14 @@
       <c r="H73" s="4"/>
       <c r="I73" s="6"/>
       <c r="J73" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" ht="14.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -2336,7 +2348,7 @@
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -2365,7 +2377,7 @@
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -2378,7 +2390,7 @@
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
@@ -2386,7 +2398,7 @@
       <c r="H78" s="11"/>
       <c r="I78" s="13"/>
       <c r="J78" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" ht="14.25">
@@ -2394,7 +2406,7 @@
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -2409,7 +2421,7 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -2423,7 +2435,7 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -2465,7 +2477,7 @@
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -2479,7 +2491,7 @@
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
@@ -2491,7 +2503,7 @@
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -2505,53 +2517,58 @@
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="4" t="s">
-        <v>110</v>
+      <c r="D87" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
-      <c r="I87" s="6"/>
-      <c r="J87" s="9"/>
+      <c r="I87" s="6">
+        <v>1</v>
+      </c>
+      <c r="J87" s="14" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="88" ht="14.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
-      <c r="D88" s="4" t="s">
-        <v>111</v>
+      <c r="D88" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="6"/>
-      <c r="J88" s="9"/>
+      <c r="J88" s="14" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="89" ht="14.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="D89" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E89" s="4"/>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="6"/>
-      <c r="J89" s="9"/>
     </row>
     <row r="90" ht="14.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="E90" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="6"/>
@@ -2564,7 +2581,7 @@
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
       <c r="F91" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
@@ -2575,11 +2592,11 @@
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
-      <c r="D92" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="D92" s="4"/>
       <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
+      <c r="F92" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="6"/>
@@ -2589,10 +2606,10 @@
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4" t="s">
-        <v>115</v>
-      </c>
+      <c r="D93" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2604,10 +2621,10 @@
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="E94" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="6"/>
@@ -2618,10 +2635,10 @@
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="6"/>
@@ -2632,10 +2649,10 @@
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="E96" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="6"/>
@@ -2646,10 +2663,10 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="6"/>
@@ -2660,10 +2677,10 @@
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="E98" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F98" s="4"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="6"/>
@@ -2674,10 +2691,10 @@
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="6"/>
@@ -2688,63 +2705,63 @@
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="E100" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="6"/>
       <c r="J100" s="9"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="11"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="10"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="9"/>
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="11"/>
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11" t="s">
-        <v>118</v>
-      </c>
+      <c r="E102" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F102" s="11"/>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
       <c r="I102" s="13"/>
       <c r="J102" s="10"/>
     </row>
     <row r="103" ht="14.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4" t="s">
+      <c r="A103" s="11"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="6"/>
-      <c r="J103" s="9"/>
+      <c r="G103" s="11"/>
+      <c r="H103" s="11"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="10"/>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -2757,10 +2774,10 @@
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="D105" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" s="4"/>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
@@ -2772,10 +2789,10 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="E106" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="6"/>
@@ -2788,7 +2805,7 @@
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -2800,16 +2817,14 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
-      <c r="E108" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="6"/>
-      <c r="J108" s="9" t="s">
-        <v>127</v>
-      </c>
+      <c r="J108" s="9"/>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="4"/>
@@ -2817,40 +2832,40 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="6"/>
       <c r="J109" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
-      <c r="D110" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
-      <c r="I110" s="6">
-        <v>1</v>
-      </c>
-      <c r="J110" s="9"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="9" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D111" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
@@ -2865,7 +2880,7 @@
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
@@ -2879,23 +2894,25 @@
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
-      <c r="D113" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="6"/>
+      <c r="I113" s="6">
+        <v>1</v>
+      </c>
       <c r="J113" s="9"/>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
-      <c r="C114" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
@@ -2906,10 +2923,10 @@
     <row r="115" ht="14.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="C115" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
@@ -2922,7 +2939,7 @@
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -2936,7 +2953,7 @@
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
@@ -2950,7 +2967,7 @@
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
@@ -2961,11 +2978,11 @@
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
-      <c r="B119" s="4" t="s">
-        <v>136</v>
-      </c>
+      <c r="B119" s="4"/>
       <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
+      <c r="D119" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
@@ -2975,21 +2992,34 @@
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="B120" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="6"/>
-      <c r="J120" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="121" ht="14.25"/>
+      <c r="J120" s="9"/>
+    </row>
+    <row r="121" ht="14.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="122" ht="14.25"/>
     <row r="123" ht="14.25"/>
   </sheetData>
@@ -3010,7 +3040,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004300E1-00FB-401A-A012-006400850052}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00160011-0003-4388-A37A-00A8001B0099}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3024,10 +3054,27 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
+          <xm:sqref>I3:I105 I106:I119 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00EE0077-0075-4B1B-8F13-0000004800CD}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{000C00AA-003A-4C60-BED6-006100870067}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I121</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004A00C7-0067-44A2-A525-0050004200C1}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3044,24 +3091,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002D000E-00A6-4931-A3B7-00D700980000}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{000B0077-0072-49E4-95A9-0030008900B9}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005300BD-0098-44CA-8867-009E006A00C9}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3078,7 +3108,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003400F7-0043-4A92-87F3-00880071005C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008F0093-009F-4C66-8846-00EB009E0072}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3095,7 +3125,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007A00CA-0084-4EEC-AB85-000E006B005F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00C90085-0094-429A-BC89-00C700840008}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3112,7 +3142,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0054009D-0026-4976-B1B4-002700D500CF}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B10084-0050-469D-8F9C-0039004400A6}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3129,7 +3159,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{005A0013-001E-440B-8EB4-00EB00D200C9}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005B00B4-00F2-4039-A913-003C000A00BE}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3146,7 +3176,7 @@
           <xm:sqref>I70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00CA0041-00E4-4857-8C25-00A600C90001}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00BE00EC-005E-404F-A824-003D00880095}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3163,7 +3193,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00060032-00F6-485B-AB85-005800E4003F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0036003A-00B9-4150-AE27-009E007100C4}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3180,7 +3210,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00140064-0053-46ED-98B6-0035009200DD}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0003005D-00EF-47C5-B91B-003600FF00B8}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3197,7 +3227,58 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001D0049-0001-4035-AC80-00260006004B}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C80049-002E-42C9-8E20-00CF006E0032}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I121</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000D00A6-0068-4C89-B3FD-00A6007F00C8}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I3:I105 I106:I119 I48:I51</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BD0051-00D4-4ACB-BD99-00EF00F60062}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A800DA-006D-4F64-A486-004E001C00BE}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3214,58 +3295,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00EE00C7-0087-4231-BF11-004600B6008B}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007A00B8-0073-4531-8A75-006600DC00B5}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0056006A-00D6-445C-9D23-008A00F80073}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003C0020-00C3-4629-9C72-006A004C0086}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00020004-0071-48BF-B374-005F003E00ED}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3282,7 +3312,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00890090-00D4-44E7-971C-00F1005F0040}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00E30048-00E4-425D-80B6-002F002B00D4}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3299,7 +3329,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BE0063-00A5-4736-A7C2-00C1007B0008}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C50053-000B-4550-B8C9-00C100BA00AC}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3316,7 +3346,7 @@
           <xm:sqref>I70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000300B8-0056-488C-A767-00AD002F00D9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00090083-00F1-48C0-B8C8-008A00420082}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3333,7 +3363,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009F00A1-000D-41B1-AFF3-003D00CD00C3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0071006E-00E6-4266-B8F7-00F5002100B7}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3350,7 +3380,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{008100A4-0072-4143-AEB2-002E00ED0069}">
+          <x14:cfRule type="dataBar" priority="2" id="{00A7005B-00FA-4713-873A-00DF00360081}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3366,7 +3396,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00BB003B-0031-4432-86D2-00F000E80081}">
+          <x14:cfRule type="dataBar" priority="1" id="{00B500C7-0086-4B2A-919C-001C00660068}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
added sensor FOV/LOS checks for image/comm payloads
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -564,7 +564,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -603,13 +603,7 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1142,7 +1136,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A80" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1203,7 +1197,7 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I119,"0")/ROWS(Table5[])</f>
-        <v>8.3333333333333332e-003</v>
+        <v>1.6666666666666666e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -2045,7 +2039,7 @@
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="6"/>
-      <c r="J56" s="14" t="s">
+      <c r="J56" s="9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2228,7 +2222,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="15">
+      <c r="I67" s="14">
         <v>1</v>
       </c>
       <c r="J67" s="9"/>
@@ -2517,7 +2511,7 @@
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="16" t="s">
+      <c r="D87" s="4" t="s">
         <v>111</v>
       </c>
       <c r="E87" s="4"/>
@@ -2527,7 +2521,7 @@
       <c r="I87" s="6">
         <v>1</v>
       </c>
-      <c r="J87" s="14" t="s">
+      <c r="J87" s="9" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2535,15 +2529,17 @@
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="4" t="s">
         <v>113</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
-      <c r="I88" s="6"/>
-      <c r="J88" s="14" t="s">
+      <c r="I88" s="6">
+        <v>0</v>
+      </c>
+      <c r="J88" s="9" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3040,7 +3036,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00160011-0003-4388-A37A-00A8001B0099}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00530049-004C-44F1-A884-00C3002700F5}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3057,7 +3053,7 @@
           <xm:sqref>I3:I105 I106:I119 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{000C00AA-003A-4C60-BED6-006100870067}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00170021-00EE-4E26-8CB3-001E002C00A0}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3074,7 +3070,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004A00C7-0067-44A2-A525-0050004200C1}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004C00F9-00BB-4B93-B59B-00F800C900F5}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3091,7 +3087,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{005300BD-0098-44CA-8867-009E006A00C9}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00110048-00B8-430D-8CCA-004B007E009E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3108,7 +3104,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008F0093-009F-4C66-8846-00EB009E0072}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008B00D7-00CB-4A1B-8693-0026007200B8}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3125,7 +3121,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C90085-0094-429A-BC89-00C700840008}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00630042-0041-4A79-808E-002D00ED0056}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3142,7 +3138,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B10084-0050-469D-8F9C-0039004400A6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0046007B-0049-4698-B016-001700DF00FF}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3159,7 +3155,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{005B00B4-00F2-4039-A913-003C000A00BE}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00650047-0076-4E1C-A0C7-002F0058002C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3176,7 +3172,7 @@
           <xm:sqref>I70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00BE00EC-005E-404F-A824-003D00880095}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F300BF-0041-425D-8306-00D3000E00CB}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3193,7 +3189,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0036003A-00B9-4150-AE27-009E007100C4}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00A900D0-0085-4AE6-8A77-00F800DB00BE}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3210,7 +3206,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0003005D-00EF-47C5-B91B-003600FF00B8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004500BC-0001-49F9-9C88-00A4003C005C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3227,7 +3223,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C80049-002E-42C9-8E20-00CF006E0032}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00060097-00DA-410A-8EE5-007200D200EF}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3244,7 +3240,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000D00A6-0068-4C89-B3FD-00A6007F00C8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003200CA-0016-453F-B601-001200E50035}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3261,7 +3257,7 @@
           <xm:sqref>I3:I105 I106:I119 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BD0051-00D4-4ACB-BD99-00EF00F60062}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00900094-0022-43F6-8394-00C700DC00DF}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3278,7 +3274,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00A800DA-006D-4F64-A486-004E001C00BE}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00EF0083-004D-473F-B517-00E700C60015}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3295,7 +3291,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00020004-0071-48BF-B374-005F003E00ED}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{009D00FF-004A-4A5D-924B-005E00D500F0}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3312,7 +3308,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00E30048-00E4-425D-80B6-002F002B00D4}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F100C0-00B2-4E4A-BBB0-002B00DD00FE}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3329,7 +3325,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C50053-000B-4550-B8C9-00C100BA00AC}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C10053-0080-4E30-890D-00E100D900C2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3346,7 +3342,7 @@
           <xm:sqref>I70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00090083-00F1-48C0-B8C8-008A00420082}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00EC009A-0094-43F1-B7EE-002700670031}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3363,7 +3359,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0071006E-00E6-4266-B8F7-00F5002100B7}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D20049-0030-4CA0-AA22-003900470036}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3380,7 +3376,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00A7005B-00FA-4713-873A-00DF00360081}">
+          <x14:cfRule type="dataBar" priority="2" id="{00D70069-007E-4D05-B439-006500E0002F}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3396,7 +3392,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00B500C7-0086-4B2A-919C-001C00660068}">
+          <x14:cfRule type="dataBar" priority="1" id="{00E400D8-0007-461D-BC0C-008F00BB006D}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Started system to generate ground points for comm missions
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>Status</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t xml:space="preserve">cone from satellite to target </t>
-  </si>
-  <si>
-    <t xml:space="preserve">take image</t>
   </si>
   <si>
     <t>experiment</t>
@@ -626,7 +623,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J121" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J120" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1136,7 +1133,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A80" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A38" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1191,13 +1188,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.26666666666666666</v>
+        <v>0.26890756302521007</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I119,"0")/ROWS(Table5[])</f>
-        <v>1.6666666666666666e-002</v>
+        <f>COUNTIF(I2:I118,"0")/ROWS(Table5[])</f>
+        <v>3.3613445378151259e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1234,7 +1231,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -2008,7 +2005,9 @@
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="6"/>
+      <c r="I54" s="6">
+        <v>0</v>
+      </c>
       <c r="J54" s="9" t="s">
         <v>70</v>
       </c>
@@ -2024,7 +2023,9 @@
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="6"/>
+      <c r="I55" s="6">
+        <v>0</v>
+      </c>
       <c r="J55" s="9"/>
     </row>
     <row r="56" ht="14.25">
@@ -2049,13 +2050,15 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4" t="s">
+      <c r="F57" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="6"/>
-      <c r="J57" s="9"/>
+      <c r="J57" s="9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="58" ht="14.25">
       <c r="A58" s="4"/>
@@ -2064,13 +2067,13 @@
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="6"/>
       <c r="J58" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" ht="14.25">
@@ -2078,32 +2081,34 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="E59" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="I59" s="6">
+        <v>1</v>
+      </c>
+      <c r="J59" s="9"/>
     </row>
     <row r="60" ht="28.5">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-      <c r="E60" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="6">
         <v>1</v>
       </c>
-      <c r="J60" s="9"/>
+      <c r="J60" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="61" ht="28.5">
       <c r="A61" s="4"/>
@@ -2112,7 +2117,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -2120,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" ht="28.5">
@@ -2130,7 +2135,7 @@
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -2138,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" ht="28.5">
@@ -2146,17 +2151,17 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="E63" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="6">
         <v>1</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" ht="28.5">
@@ -2165,7 +2170,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2174,7 +2179,7 @@
         <v>1</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" ht="14.25">
@@ -2183,33 +2188,31 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="6">
-        <v>1</v>
-      </c>
+      <c r="I65" s="6"/>
       <c r="J65" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="D66" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="6"/>
-      <c r="J66" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="I66" s="14">
+        <v>1</v>
+      </c>
+      <c r="J66" s="9"/>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" s="4"/>
@@ -2222,23 +2225,23 @@
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="14">
-        <v>1</v>
-      </c>
+      <c r="I67" s="6"/>
       <c r="J67" s="9"/>
     </row>
     <row r="68" ht="14.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="4"/>
+      <c r="E68" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
-      <c r="I68" s="6"/>
+      <c r="I68" s="6">
+        <v>1</v>
+      </c>
       <c r="J68" s="9"/>
     </row>
     <row r="69" ht="14.25">
@@ -2260,11 +2263,11 @@
     <row r="70" ht="14.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
+      <c r="C70" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="D70" s="4"/>
-      <c r="E70" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
@@ -2276,10 +2279,10 @@
     <row r="71" ht="14.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="4"/>
+      <c r="D71" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -2287,49 +2290,47 @@
       <c r="I71" s="6">
         <v>1</v>
       </c>
-      <c r="J71" s="9"/>
+      <c r="J71" s="9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
-      <c r="I72" s="6">
-        <v>1</v>
-      </c>
+      <c r="I72" s="6"/>
       <c r="J72" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="C73" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="6"/>
-      <c r="J73" s="9" t="s">
-        <v>99</v>
-      </c>
+      <c r="J73" s="9"/>
     </row>
     <row r="74" ht="14.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="4"/>
+      <c r="D74" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -2341,10 +2342,10 @@
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
@@ -2357,7 +2358,7 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -2365,44 +2366,44 @@
       <c r="I76" s="6"/>
       <c r="J76" s="9"/>
     </row>
-    <row r="77" ht="14.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4" t="s">
+    <row r="77" ht="28.5">
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="9"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="78" ht="28.5">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="10" t="s">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4" t="s">
         <v>104</v>
       </c>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="9"/>
     </row>
     <row r="79" ht="14.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="4"/>
+      <c r="E79" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
@@ -2429,7 +2430,7 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -2441,10 +2442,10 @@
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="D82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
@@ -2455,10 +2456,10 @@
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
-      <c r="D83" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
@@ -2482,11 +2483,11 @@
     <row r="85" ht="14.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
+      <c r="C85" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="D85" s="4"/>
-      <c r="E85" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -2496,33 +2497,37 @@
     <row r="86" ht="14.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="4"/>
+      <c r="D86" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
-      <c r="I86" s="6"/>
-      <c r="J86" s="9"/>
+      <c r="I86" s="6">
+        <v>1</v>
+      </c>
+      <c r="J86" s="9" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="88" ht="14.25">
@@ -2530,41 +2535,37 @@
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
-      <c r="I88" s="6">
-        <v>0</v>
-      </c>
-      <c r="J88" s="9" t="s">
-        <v>114</v>
-      </c>
+      <c r="I88" s="6"/>
     </row>
     <row r="89" ht="14.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
-      <c r="D89" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="6"/>
+      <c r="J89" s="9"/>
     </row>
     <row r="90" ht="14.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
-      <c r="E90" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="6"/>
@@ -2588,11 +2589,11 @@
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
+      <c r="D92" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="E92" s="4"/>
-      <c r="F92" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="6"/>
@@ -2602,10 +2603,10 @@
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="4"/>
+      <c r="E93" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2617,10 +2618,10 @@
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="4" t="s">
+      <c r="E94" s="4"/>
+      <c r="F94" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="6"/>
@@ -2631,10 +2632,10 @@
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4" t="s">
+      <c r="E95" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="6"/>
@@ -2645,10 +2646,10 @@
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="4" t="s">
+      <c r="E96" s="4"/>
+      <c r="F96" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="6"/>
@@ -2659,10 +2660,10 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="E97" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="6"/>
@@ -2673,10 +2674,10 @@
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="6"/>
@@ -2687,10 +2688,10 @@
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4" t="s">
+      <c r="E99" s="11" t="s">
         <v>123</v>
       </c>
+      <c r="F99" s="4"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="6"/>
@@ -2701,63 +2702,63 @@
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
-      <c r="E100" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="6"/>
       <c r="J100" s="9"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="6"/>
-      <c r="J101" s="9"/>
+      <c r="A101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F101" s="11"/>
+      <c r="G101" s="11"/>
+      <c r="H101" s="11"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="10"/>
     </row>
     <row r="102" ht="14.25">
       <c r="A102" s="11"/>
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
-      <c r="E102" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F102" s="11"/>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11" t="s">
+        <v>121</v>
+      </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
       <c r="I102" s="13"/>
       <c r="J102" s="10"/>
     </row>
     <row r="103" ht="14.25">
-      <c r="A103" s="11"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="10"/>
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="9"/>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4" t="s">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -2770,10 +2771,10 @@
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
-      <c r="D105" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
@@ -2785,10 +2786,10 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
-      <c r="E106" s="4" t="s">
+      <c r="E106" s="4"/>
+      <c r="F106" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="6"/>
@@ -2813,14 +2814,16 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4" t="s">
+      <c r="E108" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="6"/>
-      <c r="J108" s="9"/>
+      <c r="J108" s="9" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="4"/>
@@ -2828,40 +2831,40 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="6"/>
       <c r="J109" s="9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="D110" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E110" s="4"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
-      <c r="I110" s="6"/>
-      <c r="J110" s="9" t="s">
-        <v>133</v>
-      </c>
+      <c r="I110" s="6">
+        <v>1</v>
+      </c>
+      <c r="J110" s="9"/>
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
-      <c r="D111" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
@@ -2876,7 +2879,7 @@
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
@@ -2890,25 +2893,23 @@
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="D113" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="6">
-        <v>1</v>
-      </c>
+      <c r="I113" s="6"/>
       <c r="J113" s="9"/>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="C114" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D114" s="4"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
@@ -2919,10 +2920,10 @@
     <row r="115" ht="14.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
-      <c r="C115" s="4" t="s">
+      <c r="C115" s="4"/>
+      <c r="D115" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
@@ -2963,7 +2964,7 @@
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
@@ -2974,11 +2975,11 @@
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
+      <c r="B119" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="C119" s="4"/>
-      <c r="D119" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="D119" s="4"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
@@ -2988,34 +2989,21 @@
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
-      <c r="B120" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="6"/>
-      <c r="J120" s="9"/>
-    </row>
-    <row r="121" ht="14.25">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
-      <c r="I121" s="6"/>
-      <c r="J121" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
+      <c r="J120" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="121" ht="14.25"/>
     <row r="122" ht="14.25"/>
     <row r="123" ht="14.25"/>
   </sheetData>
@@ -3036,7 +3024,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00530049-004C-44F1-A884-00C3002700F5}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00980025-0080-472E-9ACF-003D002A007A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3050,27 +3038,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I105 I106:I119 I48:I51</xm:sqref>
+          <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00170021-00EE-4E26-8CB3-001E002C00A0}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I121</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004C00F9-00BB-4B93-B59B-00F800C900F5}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0046006A-0031-4E6A-9914-00170083008A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3087,7 +3058,24 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00110048-00B8-430D-8CCA-004B007E009E}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00A600AF-0022-4196-9C3F-007500DC008C}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I119</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B300CC-00E3-485A-BA99-00150020005B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3104,7 +3092,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008B00D7-00CB-4A1B-8693-0026007200B8}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00AB002C-0024-4F4F-B36E-0008001F0087}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3121,7 +3109,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00630042-0041-4A79-808E-002D00ED0056}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0092004E-003B-4483-B591-0033000D00D6}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3138,7 +3126,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0046007B-0049-4698-B016-001700DF00FF}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00AD0045-00A1-43F8-B5D2-00CE000200BE}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3155,24 +3143,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00650047-0076-4E1C-A0C7-002F0058002C}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I70</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F300BF-0041-425D-8306-00D3000E00CB}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00070038-0075-4425-958E-00E8007800EC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3189,7 +3160,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00A900D0-0085-4AE6-8A77-00F800DB00BE}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F000E3-00F8-4274-9921-00E200D000C1}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3206,7 +3177,24 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004500BC-0001-49F9-9C88-00A4003C005C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00790014-000F-4FC3-AE6B-00EF00CD00D0}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F9002F-00C4-4CE3-834F-009B00160061}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3223,7 +3211,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00060097-00DA-410A-8EE5-007200D200EF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{008A00AA-00C5-471C-AC36-004100B900F0}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3237,10 +3225,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I121</xm:sqref>
+          <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003200CA-0016-453F-B601-001200E50035}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{008C0091-00E4-44A7-9A8F-009200A300AF}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3254,10 +3242,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I105 I106:I119 I48:I51</xm:sqref>
+          <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00900094-0022-43F6-8394-00C700DC00DF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00220004-0095-4132-A34A-001500290000}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3274,7 +3262,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00EF0083-004D-473F-B517-00E700C60015}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B100B4-0073-4A60-955A-00A2008200FC}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3288,10 +3276,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I120</xm:sqref>
+          <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009D00FF-004A-4A5D-924B-005E00D500F0}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0064006A-00BC-4C46-A039-00E6004A00EF}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3308,7 +3296,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F100C0-00B2-4E4A-BBB0-002B00DD00FE}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00AA0080-00D0-4DEF-8A62-00E2000100D9}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3325,24 +3313,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C10053-0080-4E30-890D-00E100D900C2}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I70</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00EC009A-0094-43F1-B7EE-002700670031}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B50065-00B6-4DD9-B7D8-006B008A00EE}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3359,7 +3330,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D20049-0030-4CA0-AA22-003900470036}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00FD001D-0096-4E76-809D-00AC00AD0017}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3376,7 +3347,24 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00D70069-007E-4D05-B439-006500E0002F}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BC00BF-0040-42AC-973C-009F0095006F}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" priority="2" id="{007000F6-00A4-4A55-BF3F-0098005300C7}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3392,7 +3380,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00E400D8-0007-461D-BC0C-008F00BB006D}">
+          <x14:cfRule type="dataBar" priority="1" id="{005C0081-0058-4EBF-93BA-00BB00590023}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
comm msn. points initialize to surface of earth
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -363,7 +363,10 @@
     <t xml:space="preserve">lat/long for customer</t>
   </si>
   <si>
-    <t xml:space="preserve">channel/speed required</t>
+    <t>reward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list integration</t>
   </si>
   <si>
     <t xml:space="preserve">one time missions</t>
@@ -388,9 +391,6 @@
   </si>
   <si>
     <t>rendevous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$ reward based on mission difficulty</t>
   </si>
   <si>
     <t xml:space="preserve">available missions</t>
@@ -561,7 +561,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -603,6 +603,9 @@
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +626,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J120" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J130" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1133,7 +1136,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A77" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1188,13 +1191,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.26890756302521007</v>
+        <v>0.27131782945736432</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I118,"0")/ROWS(Table5[])</f>
-        <v>3.3613445378151259e-002</v>
+        <f>COUNTIF(I2:I128,"0")/ROWS(Table5[])</f>
+        <v>2.3255813953488372e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1231,7 +1234,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1266,7 +1269,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -2006,7 +2009,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" s="9" t="s">
         <v>70</v>
@@ -2524,7 +2527,7 @@
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J87" s="9" t="s">
         <v>113</v>
@@ -2554,7 +2557,9 @@
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
-      <c r="I89" s="6"/>
+      <c r="I89" s="6">
+        <v>0</v>
+      </c>
       <c r="J89" s="9"/>
     </row>
     <row r="90" ht="14.25">
@@ -2568,7 +2573,9 @@
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
-      <c r="I90" s="6"/>
+      <c r="I90" s="6">
+        <v>1</v>
+      </c>
       <c r="J90" s="9"/>
     </row>
     <row r="91" ht="14.25">
@@ -2577,7 +2584,7 @@
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
-      <c r="F91" s="4" t="s">
+      <c r="F91" s="15" t="s">
         <v>116</v>
       </c>
       <c r="G91" s="4"/>
@@ -2589,11 +2596,11 @@
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="6"/>
@@ -2603,10 +2610,10 @@
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4" t="s">
+      <c r="D93" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2618,10 +2625,10 @@
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4" t="s">
+      <c r="E94" s="4" t="s">
         <v>119</v>
       </c>
+      <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="6"/>
@@ -2632,10 +2639,10 @@
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="4" t="s">
+      <c r="E95" s="4"/>
+      <c r="F95" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="6"/>
@@ -2648,7 +2655,7 @@
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
@@ -2660,10 +2667,10 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="6"/>
@@ -2674,10 +2681,10 @@
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="E98" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F98" s="4"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="6"/>
@@ -2688,10 +2695,10 @@
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="15" t="s">
+        <v>122</v>
+      </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="6"/>
@@ -2704,7 +2711,7 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
@@ -2712,42 +2719,42 @@
       <c r="J100" s="9"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="11"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="10"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="9"/>
     </row>
     <row r="102" ht="14.25">
-      <c r="A102" s="11"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="10"/>
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="9"/>
     </row>
     <row r="103" ht="14.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
-      <c r="D103" s="4" t="s">
-        <v>125</v>
-      </c>
+      <c r="D103" s="4"/>
       <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
+      <c r="F103" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="6"/>
@@ -2757,11 +2764,11 @@
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
-      <c r="D104" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D104" s="4"/>
       <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
+      <c r="F104" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="6"/>
@@ -2772,10 +2779,10 @@
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
-      <c r="E105" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="6"/>
@@ -2786,10 +2793,10 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="E106" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="6"/>
@@ -2802,7 +2809,7 @@
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -2814,90 +2821,80 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
-      <c r="E108" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="6"/>
-      <c r="J108" s="9" t="s">
-        <v>130</v>
-      </c>
+      <c r="J108" s="9"/>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
-      <c r="E109" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="6"/>
-      <c r="J109" s="9" t="s">
-        <v>132</v>
-      </c>
+      <c r="J109" s="9"/>
     </row>
     <row r="110" ht="14.25">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="6">
-        <v>1</v>
-      </c>
-      <c r="J110" s="9"/>
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F110" s="11"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="10"/>
     </row>
     <row r="111" ht="14.25">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
-      <c r="I111" s="6">
-        <v>1</v>
-      </c>
-      <c r="J111" s="9"/>
+      <c r="A111" s="11"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="G111" s="11"/>
+      <c r="H111" s="11"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="10"/>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
-      <c r="E112" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
-      <c r="I112" s="6">
-        <v>1</v>
-      </c>
+      <c r="I112" s="6"/>
       <c r="J112" s="9"/>
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
-      <c r="D113" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="D113" s="4"/>
       <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
+      <c r="F113" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
       <c r="I113" s="6"/>
@@ -2906,10 +2903,10 @@
     <row r="114" ht="14.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
-      <c r="C114" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
@@ -2921,10 +2918,10 @@
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
-      <c r="D115" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
@@ -2935,11 +2932,11 @@
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
-      <c r="D116" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="D116" s="4"/>
       <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
+      <c r="F116" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="6"/>
@@ -2949,11 +2946,11 @@
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
-      <c r="D117" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="D117" s="4"/>
       <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
+      <c r="F117" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="6"/>
@@ -2963,49 +2960,196 @@
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
-      <c r="D118" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="9"/>
+      <c r="J118" s="9" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
-      <c r="B119" s="4" t="s">
-        <v>139</v>
-      </c>
+      <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
+      <c r="E119" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="6"/>
-      <c r="J119" s="9"/>
+      <c r="J119" s="9" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
-      <c r="I120" s="6"/>
-      <c r="J120" s="9" t="s">
+      <c r="I120" s="6">
+        <v>1</v>
+      </c>
+      <c r="J120" s="9"/>
+    </row>
+    <row r="121" ht="14.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4"/>
+      <c r="I121" s="6">
+        <v>1</v>
+      </c>
+      <c r="J121" s="9"/>
+    </row>
+    <row r="122" ht="14.25">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="6">
+        <v>1</v>
+      </c>
+      <c r="J122" s="9"/>
+    </row>
+    <row r="123" ht="14.25">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="9"/>
+    </row>
+    <row r="124" ht="14.25">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="6"/>
+      <c r="J124" s="9"/>
+    </row>
+    <row r="125" ht="14.25">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="6"/>
+      <c r="J125" s="9"/>
+    </row>
+    <row r="126" ht="14.25">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="9"/>
+    </row>
+    <row r="127" ht="14.25">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+      <c r="H127" s="4"/>
+      <c r="I127" s="6"/>
+      <c r="J127" s="9"/>
+    </row>
+    <row r="128" ht="14.25">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="6"/>
+      <c r="J128" s="9"/>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="9"/>
+    </row>
+    <row r="130" ht="14.25">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="4"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="121" ht="14.25"/>
-    <row r="122" ht="14.25"/>
-    <row r="123" ht="14.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
@@ -3024,7 +3168,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00980025-0080-472E-9ACF-003D002A007A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00FE00BD-006C-4F6B-9ECD-00B100E400F8}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3038,10 +3182,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
+          <xm:sqref>I3:I114 I115:I128 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0046006A-0031-4E6A-9914-00170083008A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003000F4-006D-4CE4-B418-00460015000F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3055,10 +3199,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I120</xm:sqref>
+          <xm:sqref>I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00A600AF-0022-4196-9C3F-007500DC008C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00420086-00A5-4F12-8D1E-002F006B0074}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3072,10 +3216,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
+          <xm:sqref>I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B300CC-00E3-485A-BA99-00150020005B}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00510096-0035-4E14-B2A8-005200C40060}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3092,7 +3236,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00AB002C-0024-4F4F-B36E-0008001F0087}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00FB0019-00A1-4D3E-99C9-002A002200FB}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3109,7 +3253,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0092004E-003B-4483-B591-0033000D00D6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E80057-004F-4F98-B24D-0047002B00E4}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3126,7 +3270,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00AD0045-00A1-43F8-B5D2-00CE000200BE}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003E006D-000C-4C5F-8551-00CB00A700AC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3143,7 +3287,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00070038-0075-4425-958E-00E8007800EC}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{002B00CE-0086-4382-A3AB-00EE0006005B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3160,7 +3304,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F000E3-00F8-4274-9921-00E200D000C1}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005F00BD-00D3-4226-A47D-007B00D800EA}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3177,7 +3321,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00790014-000F-4FC3-AE6B-00EF00CD00D0}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008F00D5-00E9-4723-B3A6-0051005300C8}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3194,7 +3338,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F9002F-00C4-4CE3-834F-009B00160061}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F30081-0023-4786-B051-00E400D00056}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3211,7 +3355,7 @@
           <xm:sqref>I29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008A00AA-00C5-471C-AC36-004100B900F0}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90084-00C3-430D-9B65-00B9004E006A}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3225,10 +3369,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I120</xm:sqref>
+          <xm:sqref>I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008C0091-00E4-44A7-9A8F-009200A300AF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D00072-006A-48AD-9612-00ED00EE00CF}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3242,10 +3386,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I104 I105:I118 I48:I51</xm:sqref>
+          <xm:sqref>I3:I114 I115:I128 I48:I51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00220004-0095-4132-A34A-001500290000}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00CD0035-00A1-4B0F-B04A-00AE007500C3}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3262,7 +3406,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B100B4-0073-4A60-955A-00A2008200FC}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000A008A-0054-450F-8745-00C000CD0078}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3276,10 +3420,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
+          <xm:sqref>I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0064006A-00BC-4C46-A039-00E6004A00EF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D20081-0052-4E3C-B3FC-00F900840094}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3296,7 +3440,7 @@
           <xm:sqref>I30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AA0080-00D0-4DEF-8A62-00E2000100D9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F60000-00CE-4F5B-89B0-00C6004B00B1}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3313,7 +3457,7 @@
           <xm:sqref>I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B50065-00B6-4DD9-B7D8-006B008A00EE}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004C0041-00E1-46E4-A460-00A4007900DE}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3330,7 +3474,7 @@
           <xm:sqref>I69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00FD001D-0096-4E76-809D-00AC00AD0017}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{002A004F-0006-4D83-8756-00A70086001C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3347,7 +3491,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BC00BF-0040-42AC-973C-009F0095006F}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00EF008D-009C-4A97-8B9C-00F7009000E2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3364,7 +3508,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{007000F6-00A4-4A55-BF3F-0098005300C7}">
+          <x14:cfRule type="dataBar" priority="2" id="{007B002F-0067-48B7-9E7D-004E00D90099}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3380,7 +3524,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{005C0081-0058-4EBF-93BA-00BB00590023}">
+          <x14:cfRule type="dataBar" priority="1" id="{00B100BF-0010-4A28-9012-007C00470020}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
moved to URP, reimported assets, added FOV display
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -81,9 +81,6 @@
     <t xml:space="preserve">exit program</t>
   </si>
   <si>
-    <t>Integration</t>
-  </si>
-  <si>
     <t>Background</t>
   </si>
   <si>
@@ -228,13 +225,22 @@
     <t>passive</t>
   </si>
   <si>
+    <t xml:space="preserve">show beam coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">must check if view is limited by sensor area or horizon</t>
+  </si>
+  <si>
     <t>imagery</t>
   </si>
   <si>
-    <t xml:space="preserve">show area to image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cone from satellite to target </t>
+    <t xml:space="preserve">mission must be in footprint, cooldown timer on completing missions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show imagery area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy FOV from data relay</t>
   </si>
   <si>
     <t>experiment</t>
@@ -357,10 +363,7 @@
     <t xml:space="preserve">chance for each mission type</t>
   </si>
   <si>
-    <t xml:space="preserve">continuous missions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat/long for customer</t>
+    <t xml:space="preserve">initialize points</t>
   </si>
   <si>
     <t>reward</t>
@@ -369,9 +372,6 @@
     <t xml:space="preserve">list integration</t>
   </si>
   <si>
-    <t xml:space="preserve">one time missions</t>
-  </si>
-  <si>
     <t xml:space="preserve">ground imagery</t>
   </si>
   <si>
@@ -396,22 +396,13 @@
     <t xml:space="preserve">available missions</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add to active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">active missions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">completed artwork/design</t>
-  </si>
-  <si>
-    <t>completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">basic buttons</t>
+    <t xml:space="preserve">missions are added to list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select to view parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show points when selected</t>
   </si>
   <si>
     <t>Time-scaling</t>
@@ -436,6 +427,15 @@
   </si>
   <si>
     <t xml:space="preserve">80/90s asthetic - win95 style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactor/Performance Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cache GetComponent&lt;&gt;() calls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduce the number of GetComponent calls as much as possible</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,7 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -552,6 +552,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -561,7 +579,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -600,11 +618,17 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -626,7 +650,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J130" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J127" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1136,7 +1160,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1191,13 +1215,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.27131782945736432</v>
+        <v>0.29365079365079366</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I128,"0")/ROWS(Table5[])</f>
-        <v>2.3255813953488372e-002</v>
+        <f>COUNTIF(I2:I123,"0")/ROWS(Table5[])</f>
+        <v>1.5873015873015872e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1234,7 +1258,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1269,7 +1293,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1471,10 +1495,10 @@
     <row r="21" ht="14.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1498,10 +1522,10 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1510,174 +1534,174 @@
       <c r="I23" s="6"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" ht="14.25">
+    <row r="24" ht="28.5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" ht="14.25">
+      <c r="I24" s="6">
+        <v>1</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" ht="28.5">
       <c r="A25" s="4"/>
-      <c r="B25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="9"/>
+      <c r="J25" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" ht="28.5">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="6">
-        <v>1</v>
-      </c>
+      <c r="I26" s="6"/>
       <c r="J26" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="6"/>
+      <c r="I27" s="6">
+        <v>1</v>
+      </c>
       <c r="J27" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="C28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="I28" s="6">
+        <v>1</v>
+      </c>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="6">
-        <v>1</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="9"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="6">
-        <v>1</v>
-      </c>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" ht="14.25">
+      <c r="I30" s="6"/>
+      <c r="J30" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" ht="28.5">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="9"/>
+      <c r="I31" s="6">
+        <v>1</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="6">
-        <v>0</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" ht="28.5">
+        <v>1</v>
+      </c>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" ht="14.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="6">
-        <v>1</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25">
+      <c r="I33" s="6"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" ht="28.5">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1686,69 +1710,73 @@
       <c r="I34" s="6">
         <v>1</v>
       </c>
-      <c r="J34" s="9"/>
-    </row>
-    <row r="35" ht="28.5">
+      <c r="J34" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="6"/>
-      <c r="J35" s="9"/>
-    </row>
-    <row r="36" ht="28.5">
+      <c r="J35" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="6">
-        <v>1</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="9"/>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="6"/>
       <c r="J37" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="9"/>
+      <c r="I38" s="6">
+        <v>1</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="4"/>
@@ -1756,42 +1784,38 @@
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="I39" s="6">
+        <v>1</v>
+      </c>
+      <c r="J39" s="9"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="C40" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="6">
-        <v>1</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>49</v>
-      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="9"/>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="D41" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -1803,120 +1827,126 @@
     <row r="42" ht="14.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="6"/>
+      <c r="I42" s="6">
+        <v>1</v>
+      </c>
       <c r="J42" s="9"/>
     </row>
     <row r="43" ht="28.5">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="11" t="s">
-        <v>52</v>
+      <c r="D43" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="6">
+      <c r="I43" s="12">
         <v>1</v>
       </c>
       <c r="J43" s="9"/>
     </row>
     <row r="44" ht="28.5">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="6">
-        <v>1</v>
-      </c>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" ht="28.5">
+        <v>54</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="13">
+        <v>1</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="12">
-        <v>1</v>
-      </c>
+      <c r="I45" s="6"/>
       <c r="J45" s="9"/>
     </row>
-    <row r="46" ht="28.5">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="13">
-        <v>1</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>56</v>
-      </c>
+    <row r="46" ht="14.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="6">
+        <v>1</v>
+      </c>
+      <c r="J46" s="9"/>
     </row>
     <row r="47" ht="28.5">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
-      <c r="D47" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="D47" s="4"/>
       <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
+      <c r="F47" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="9"/>
+      <c r="I47" s="6">
+        <v>1</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="48" ht="28.5">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="6">
         <v>1</v>
       </c>
-      <c r="J48" s="9"/>
-    </row>
-    <row r="49" ht="28.5">
+      <c r="J48" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -1924,61 +1954,61 @@
         <v>1</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" ht="28.5">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="6">
-        <v>1</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" ht="28.5">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="13">
+        <v>1</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="E51" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" ht="28.5">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="13">
-        <v>1</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" ht="14.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="6">
+        <v>1</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="53" ht="28.5">
@@ -1986,33 +2016,33 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
-      <c r="E53" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25">
+      <c r="I53" s="6">
+        <v>1</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" ht="28.5">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="6">
-        <v>1</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>70</v>
+      <c r="I54" s="6"/>
+      <c r="J54" s="14" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="55" ht="14.25">
@@ -2022,14 +2052,16 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="6">
         <v>0</v>
       </c>
-      <c r="J55" s="9"/>
+      <c r="J55" s="14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="56" ht="14.25">
       <c r="A56" s="4"/>
@@ -2037,14 +2069,14 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="F56" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="6"/>
       <c r="J56" s="9" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" ht="14.25">
@@ -2054,13 +2086,13 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="6"/>
       <c r="J57" s="9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" ht="14.25">
@@ -2068,32 +2100,34 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="E58" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" ht="14.25">
+      <c r="I58" s="6">
+        <v>1</v>
+      </c>
+      <c r="J58" s="9"/>
+    </row>
+    <row r="59" ht="28.5">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="6">
         <v>1</v>
       </c>
-      <c r="J59" s="9"/>
+      <c r="J59" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="60" ht="28.5">
       <c r="A60" s="4"/>
@@ -2102,7 +2136,7 @@
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -2110,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" ht="28.5">
@@ -2120,7 +2154,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -2128,34 +2162,34 @@
         <v>1</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" ht="28.5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" ht="14.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="E62" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="6">
         <v>1</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" ht="28.5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" ht="14.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2164,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" ht="28.5">
@@ -2173,62 +2207,60 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
-      <c r="I64" s="6">
-        <v>1</v>
-      </c>
+      <c r="I64" s="6"/>
       <c r="J64" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="D65" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="I65" s="15">
+        <v>1</v>
+      </c>
+      <c r="J65" s="9"/>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="14">
-        <v>1</v>
-      </c>
+      <c r="I66" s="6"/>
       <c r="J66" s="9"/>
     </row>
     <row r="67" ht="14.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="D67" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="6"/>
+      <c r="I67" s="6">
+        <v>1</v>
+      </c>
       <c r="J67" s="9"/>
     </row>
     <row r="68" ht="14.25">
@@ -2237,7 +2269,7 @@
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -2250,11 +2282,11 @@
     <row r="69" ht="14.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
+      <c r="C69" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="D69" s="4"/>
-      <c r="E69" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -2266,10 +2298,10 @@
     <row r="70" ht="14.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -2277,49 +2309,47 @@
       <c r="I70" s="6">
         <v>1</v>
       </c>
-      <c r="J70" s="9"/>
+      <c r="J70" s="9" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
-      <c r="I71" s="6">
-        <v>1</v>
-      </c>
+      <c r="I71" s="6"/>
       <c r="J71" s="9" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="C72" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="6"/>
-      <c r="J72" s="9" t="s">
-        <v>98</v>
-      </c>
+      <c r="J72" s="9"/>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -2331,10 +2361,10 @@
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -2347,7 +2377,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -2356,43 +2386,43 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" ht="14.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="9"/>
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="77" ht="28.5">
-      <c r="A77" s="11"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="9"/>
     </row>
     <row r="78" ht="28.5">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
-      <c r="D78" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
@@ -2405,7 +2435,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -2419,7 +2449,7 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -2431,10 +2461,10 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="D81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="4"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
@@ -2445,10 +2475,10 @@
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
-      <c r="D82" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
@@ -2461,7 +2491,7 @@
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -2472,11 +2502,11 @@
     <row r="84" ht="14.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
+      <c r="C84" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="D84" s="4"/>
-      <c r="E84" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
@@ -2486,23 +2516,27 @@
     <row r="85" ht="14.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
-      <c r="C85" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
-      <c r="I85" s="6"/>
-      <c r="J85" s="9"/>
+      <c r="I85" s="6">
+        <v>1</v>
+      </c>
+      <c r="J85" s="9" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -2512,53 +2546,52 @@
         <v>1</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
-      <c r="I87" s="6">
-        <v>1</v>
-      </c>
-      <c r="J87" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="I87" s="6"/>
+      <c r="J87" s="9"/>
     </row>
     <row r="88" ht="14.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
-      <c r="D88" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="D88" s="4"/>
       <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
+      <c r="F88" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
-      <c r="I88" s="6"/>
+      <c r="I88" s="6">
+        <v>1</v>
+      </c>
+      <c r="J88" s="9"/>
     </row>
     <row r="89" ht="14.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
-      <c r="E89" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J89" s="9"/>
     </row>
@@ -2569,13 +2602,11 @@
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
-      <c r="I90" s="6">
-        <v>1</v>
-      </c>
+      <c r="I90" s="6"/>
       <c r="J90" s="9"/>
     </row>
     <row r="91" ht="14.25">
@@ -2583,10 +2614,10 @@
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="15" t="s">
-        <v>116</v>
-      </c>
+      <c r="E91" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="6"/>
@@ -2598,8 +2629,8 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
-      <c r="F92" s="15" t="s">
-        <v>117</v>
+      <c r="F92" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
@@ -2610,11 +2641,11 @@
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
-      <c r="D93" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="D93" s="4"/>
       <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
+      <c r="F93" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="6"/>
@@ -2625,10 +2656,10 @@
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="6"/>
@@ -2639,10 +2670,10 @@
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4" t="s">
-        <v>120</v>
-      </c>
+      <c r="E95" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="6"/>
@@ -2655,7 +2686,7 @@
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
@@ -2681,10 +2712,10 @@
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="6"/>
@@ -2695,10 +2726,10 @@
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="15" t="s">
-        <v>122</v>
-      </c>
+      <c r="E99" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F99" s="4"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="6"/>
@@ -2711,7 +2742,7 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
@@ -2737,10 +2768,10 @@
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
-      <c r="E102" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="6"/>
@@ -2751,10 +2782,10 @@
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="E103" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="6"/>
@@ -2767,7 +2798,7 @@
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
@@ -2793,42 +2824,42 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
-      <c r="E106" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="6"/>
       <c r="J106" s="9"/>
     </row>
     <row r="107" ht="14.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4" t="s">
+      <c r="A107" s="11"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="10"/>
+    </row>
+    <row r="108" ht="14.25">
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
-      <c r="I107" s="6"/>
-      <c r="J107" s="9"/>
-    </row>
-    <row r="108" ht="14.25">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
-      <c r="I108" s="6"/>
-      <c r="J108" s="9"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="10"/>
     </row>
     <row r="109" ht="14.25">
       <c r="A109" s="4"/>
@@ -2845,42 +2876,42 @@
       <c r="J109" s="9"/>
     </row>
     <row r="110" ht="14.25">
-      <c r="A110" s="11"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F110" s="11"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="13"/>
-      <c r="J110" s="10"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="9"/>
     </row>
     <row r="111" ht="14.25">
-      <c r="A111" s="11"/>
-      <c r="B111" s="11"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="10"/>
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="9"/>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="E112" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="6"/>
@@ -2893,7 +2924,7 @@
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
@@ -2904,11 +2935,11 @@
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
-      <c r="D114" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D114" s="4"/>
       <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
+      <c r="F114" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="6"/>
@@ -2919,10 +2950,10 @@
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
-      <c r="E115" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="6"/>
@@ -2932,14 +2963,16 @@
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
+      <c r="D116" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="E116" s="4"/>
-      <c r="F116" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
-      <c r="I116" s="6"/>
+      <c r="I116" s="6">
+        <v>1</v>
+      </c>
       <c r="J116" s="9"/>
     </row>
     <row r="117" ht="14.25">
@@ -2947,13 +2980,15 @@
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4" t="s">
-        <v>128</v>
-      </c>
+      <c r="E117" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
-      <c r="I117" s="6"/>
+      <c r="I117" s="6">
+        <v>1</v>
+      </c>
       <c r="J117" s="9"/>
     </row>
     <row r="118" ht="14.25">
@@ -2962,31 +2997,29 @@
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
-      <c r="I118" s="6"/>
-      <c r="J118" s="9" t="s">
-        <v>130</v>
-      </c>
+      <c r="I118" s="6">
+        <v>1</v>
+      </c>
+      <c r="J118" s="9"/>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
+      <c r="C119" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D119" s="4"/>
-      <c r="E119" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="6"/>
-      <c r="J119" s="9" t="s">
-        <v>132</v>
-      </c>
+      <c r="J119" s="9"/>
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
@@ -2999,41 +3032,35 @@
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
-      <c r="I120" s="6">
-        <v>1</v>
-      </c>
+      <c r="I120" s="6"/>
       <c r="J120" s="9"/>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D121" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E121" s="4"/>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
-      <c r="I121" s="6">
-        <v>1</v>
-      </c>
+      <c r="I121" s="6"/>
       <c r="J121" s="9"/>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="D122" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E122" s="4"/>
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
-      <c r="I122" s="6">
-        <v>1</v>
-      </c>
+      <c r="I122" s="6"/>
       <c r="J122" s="9"/>
     </row>
     <row r="123" ht="14.25">
@@ -3041,7 +3068,7 @@
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
@@ -3052,10 +3079,10 @@
     </row>
     <row r="124" ht="14.25">
       <c r="A124" s="4"/>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="B124" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
@@ -3067,89 +3094,45 @@
     <row r="125" ht="14.25">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4" t="s">
-        <v>136</v>
-      </c>
+      <c r="C125" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D125" s="4"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="6"/>
-      <c r="J125" s="9"/>
+      <c r="J125" s="9" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="126" ht="14.25">
       <c r="A126" s="4"/>
-      <c r="B126" s="4"/>
+      <c r="B126" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="C126" s="4"/>
-      <c r="D126" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="D126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
-      <c r="H126" s="4"/>
+      <c r="H126" s="16"/>
       <c r="I126" s="6"/>
-      <c r="J126" s="9"/>
+      <c r="J126" s="17"/>
     </row>
     <row r="127" ht="14.25">
-      <c r="A127" s="4"/>
-      <c r="B127" s="4"/>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E127" s="4"/>
-      <c r="F127" s="4"/>
-      <c r="G127" s="4"/>
-      <c r="H127" s="4"/>
+      <c r="C127" t="s">
+        <v>139</v>
+      </c>
       <c r="I127" s="6"/>
-      <c r="J127" s="9"/>
-    </row>
-    <row r="128" ht="14.25">
-      <c r="A128" s="4"/>
-      <c r="B128" s="4"/>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E128" s="4"/>
-      <c r="F128" s="4"/>
-      <c r="G128" s="4"/>
-      <c r="H128" s="4"/>
-      <c r="I128" s="6"/>
-      <c r="J128" s="9"/>
-    </row>
-    <row r="129" ht="14.25">
-      <c r="A129" s="4"/>
-      <c r="B129" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C129" s="4"/>
-      <c r="D129" s="4"/>
-      <c r="E129" s="4"/>
-      <c r="F129" s="4"/>
-      <c r="G129" s="4"/>
-      <c r="H129" s="4"/>
-      <c r="I129" s="6"/>
-      <c r="J129" s="9"/>
-    </row>
-    <row r="130" ht="14.25">
-      <c r="A130" s="4"/>
-      <c r="B130" s="4"/>
-      <c r="C130" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D130" s="4"/>
-      <c r="E130" s="4"/>
-      <c r="F130" s="4"/>
-      <c r="G130" s="4"/>
-      <c r="H130" s="4"/>
-      <c r="I130" s="6"/>
-      <c r="J130" s="9" t="s">
+      <c r="J127" t="s">
         <v>140</v>
       </c>
     </row>
+    <row r="128" ht="14.25"/>
+    <row r="129" ht="14.25"/>
+    <row r="130" ht="14.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
@@ -3168,7 +3151,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00FE00BD-006C-4F6B-9ECD-00B100E400F8}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008400A8-009F-49A3-A138-003900230050}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3182,10 +3165,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I114 I115:I128 I48:I51</xm:sqref>
+          <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003000F4-006D-4CE4-B418-00460015000F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007F0049-007B-4B45-80DE-007200A4003B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3199,10 +3182,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I130</xm:sqref>
+          <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00420086-00A5-4F12-8D1E-002F006B0074}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00360003-00C0-4011-8CB3-00DC00C50027}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3216,10 +3199,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I129</xm:sqref>
+          <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00510096-0035-4E14-B2A8-005200C40060}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0091005D-0016-41F8-B2E5-003D00C600D4}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3233,10 +3216,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I30</xm:sqref>
+          <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00FB0019-00A1-4D3E-99C9-002A002200FB}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004F0042-005A-4831-8D37-008000D70008}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3250,10 +3233,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I29</xm:sqref>
+          <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E80057-004F-4F98-B24D-0047002B00E4}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007E0083-001C-45B7-9181-003200A0000C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3270,7 +3253,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003E006D-000C-4C5F-8551-00CB00A700AC}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00060052-001F-47C8-922D-000400B9002A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3284,27 +3267,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I46</xm:sqref>
+          <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002B00CE-0086-4382-A3AB-00EE0006005B}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I69</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{005F00BD-00D3-4226-A47D-007B00D800EA}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{001F00C7-00DC-4468-8EBC-004B00320035}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3321,7 +3287,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008F00D5-00E9-4723-B3A6-0051005300C8}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D6005E-0000-48DC-9441-0083000D0001}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3338,7 +3304,58 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F30081-0023-4786-B051-00E400D00056}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008C0077-00E9-482F-ADE1-00C800BF00E6}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007700D5-002D-49B1-A558-005B00B30041}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{001F0020-0013-4772-9376-002400C700F3}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I127</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00E20063-0018-4CCB-809E-002A00CC00E0}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3352,10 +3369,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I29</xm:sqref>
+          <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90084-00C3-430D-9B65-00B9004E006A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0071008E-006B-44D6-9546-001C000A0072}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3369,10 +3386,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I130</xm:sqref>
+          <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D00072-006A-48AD-9612-00ED00EE00CF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005000F5-0071-48F1-9A7B-00CB00BA0014}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3386,10 +3403,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I114 I115:I128 I48:I51</xm:sqref>
+          <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00CD0035-00A1-4B0F-B04A-00AE007500C3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005A00CF-0042-4F40-8A5A-00AE008A00B7}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3406,7 +3423,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000A008A-0054-450F-8745-00C000CD0078}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003B00B9-002A-4928-B097-005D001D0050}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3420,10 +3437,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I129</xm:sqref>
+          <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D20081-0052-4E3C-B3FC-00F900840094}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F40030-0029-41D4-9AFA-001600880057}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3437,10 +3454,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I30</xm:sqref>
+          <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F60000-00CE-4F5B-89B0-00C6004B00B1}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005B001A-0073-4CB3-99DD-003C00D6004A}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3454,27 +3471,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I46</xm:sqref>
+          <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004C0041-00E1-46E4-A460-00A4007900DE}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I69</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{002A004F-0006-4D83-8756-00A70086001C}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0098003E-00F1-43F7-90AF-00D200850028}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3491,7 +3491,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00EF008D-009C-4A97-8B9C-00F7009000E2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A900C8-00BE-4718-9675-0004000600F7}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3508,7 +3508,58 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{007B002F-0067-48B7-9E7D-004E00D90099}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00DF00C6-00AB-4950-A644-009F0041003E}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005E00AD-00BC-401D-9FC8-0094000F008B}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A100D4-00A9-41C2-97C0-007900BF00EF}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I127</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" priority="2" id="{00F400F7-005D-43C5-B87F-00070092007D}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3524,7 +3575,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00B100BF-0010-4A28-9012-007C00470020}">
+          <x14:cfRule type="dataBar" priority="1" id="{00F800B6-007A-4972-B26C-009D003E00CF}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
added image payloads & fov display for them
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Status</t>
   </si>
@@ -375,6 +375,9 @@
     <t xml:space="preserve">ground imagery</t>
   </si>
   <si>
+    <t xml:space="preserve">copy from data relay, only 1 point</t>
+  </si>
+  <si>
     <t>lat/long</t>
   </si>
   <si>
@@ -427,6 +430,12 @@
   </si>
   <si>
     <t xml:space="preserve">80/90s asthetic - win95 style</t>
+  </si>
+  <si>
+    <t>lighting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dark side of earth needs to be visible</t>
   </si>
   <si>
     <t xml:space="preserve">Refactor/Performance Pass</t>
@@ -618,9 +627,6 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -630,6 +636,7 @@
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,7 +657,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J127" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J128" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1215,13 +1222,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.29365079365079366</v>
+        <v>0.29921259842519687</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I123,"0")/ROWS(Table5[])</f>
-        <v>1.5873015873015872e-002</v>
+        <v>2.3622047244094488e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1258,7 +1265,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1293,7 +1300,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1986,9 +1993,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-      <c r="I51" s="6">
-        <v>0</v>
-      </c>
+      <c r="I51" s="6"/>
       <c r="J51" s="9" t="s">
         <v>67</v>
       </c>
@@ -2025,7 +2030,7 @@
       <c r="I53" s="6">
         <v>1</v>
       </c>
-      <c r="J53" s="14" t="s">
+      <c r="J53" s="9" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2041,7 +2046,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="6"/>
-      <c r="J54" s="14" t="s">
+      <c r="J54" s="9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2057,9 +2062,9 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="6">
-        <v>0</v>
-      </c>
-      <c r="J55" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" s="9" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2228,7 +2233,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="15">
+      <c r="I65" s="14">
         <v>1</v>
       </c>
       <c r="J65" s="9"/>
@@ -2620,8 +2625,12 @@
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
-      <c r="I91" s="6"/>
-      <c r="J91" s="9"/>
+      <c r="I91" s="6">
+        <v>0</v>
+      </c>
+      <c r="J91" s="9" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="4"/>
@@ -2630,11 +2639,13 @@
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
       <c r="F92" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
-      <c r="I92" s="6"/>
+      <c r="I92" s="6">
+        <v>0</v>
+      </c>
       <c r="J92" s="9"/>
     </row>
     <row r="93" ht="14.25">
@@ -2648,7 +2659,9 @@
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
-      <c r="I93" s="6"/>
+      <c r="I93" s="6">
+        <v>0</v>
+      </c>
       <c r="J93" s="9"/>
     </row>
     <row r="94" ht="14.25">
@@ -2671,7 +2684,7 @@
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
@@ -2686,7 +2699,7 @@
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
@@ -2742,7 +2755,7 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
@@ -2783,7 +2796,7 @@
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
@@ -2798,7 +2811,7 @@
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
@@ -2839,7 +2852,7 @@
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F107" s="11"/>
       <c r="G107" s="11"/>
@@ -2854,7 +2867,7 @@
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
       <c r="F108" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
@@ -2909,7 +2922,7 @@
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
@@ -2924,7 +2937,7 @@
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
@@ -2938,7 +2951,7 @@
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
@@ -2952,7 +2965,7 @@
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
@@ -2964,7 +2977,7 @@
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -2997,7 +3010,7 @@
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
@@ -3011,7 +3024,7 @@
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -3026,7 +3039,7 @@
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
@@ -3040,7 +3053,7 @@
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
@@ -3054,7 +3067,7 @@
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
@@ -3080,7 +3093,7 @@
     <row r="124" ht="14.25">
       <c r="A124" s="4"/>
       <c r="B124" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
@@ -3104,34 +3117,53 @@
       <c r="H125" s="4"/>
       <c r="I125" s="6"/>
       <c r="J125" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="126" ht="14.25">
       <c r="A126" s="4"/>
-      <c r="B126" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
-      <c r="H126" s="16"/>
+      <c r="H126" s="4"/>
       <c r="I126" s="6"/>
-      <c r="J126" s="17"/>
+      <c r="J126" s="9" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="127" ht="14.25">
-      <c r="C127" t="s">
-        <v>139</v>
-      </c>
+      <c r="A127" s="4"/>
+      <c r="B127" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="4"/>
+      <c r="G127" s="4"/>
+      <c r="H127" s="15"/>
       <c r="I127" s="6"/>
-      <c r="J127" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="128" ht="14.25"/>
-    <row r="129" ht="14.25"/>
+      <c r="J127" s="16"/>
+    </row>
+    <row r="128" ht="14.25">
+      <c r="C128" t="s">
+        <v>142</v>
+      </c>
+      <c r="I128" s="6"/>
+      <c r="J128" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="C129" s="17"/>
+      <c r="I129" s="4"/>
+      <c r="J129" s="17"/>
+    </row>
     <row r="130" ht="14.25"/>
   </sheetData>
   <mergeCells count="4">
@@ -3151,7 +3183,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008400A8-009F-49A3-A138-003900230050}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{002D0065-003C-4D28-8EC3-000A00280039}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3168,7 +3200,7 @@
           <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007F0049-007B-4B45-80DE-007200A4003B}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00DA0000-0025-4818-A4C2-0054003E00BE}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3185,7 +3217,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00360003-00C0-4011-8CB3-00DC00C50027}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007100AE-00AF-48D4-A39A-004C00AB00BD}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3202,7 +3234,7 @@
           <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0091005D-0016-41F8-B2E5-003D00C600D4}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{009C000C-0079-4FFB-BDE8-003E00D70094}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3219,7 +3251,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004F0042-005A-4831-8D37-008000D70008}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0078003B-00FA-4C92-8184-00B700BC00C3}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3236,7 +3268,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007E0083-001C-45B7-9181-003200A0000C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00190060-00FB-4E7F-ABF5-000B00690071}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3253,7 +3285,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00060052-001F-47C8-922D-000400B9002A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00030022-0018-490F-8EF4-00D0008200E6}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3270,7 +3302,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{001F00C7-00DC-4468-8EBC-004B00320035}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B2002F-0043-4571-84F5-006100BE0012}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3287,7 +3319,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D6005E-0000-48DC-9441-0083000D0001}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{001300B7-0041-4538-B59C-005C00680005}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3304,7 +3336,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008C0077-00E9-482F-ADE1-00C800BF00E6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{000800EF-002B-44DD-AA3F-002400DE0075}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3321,24 +3353,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007700D5-002D-49B1-A558-005B00B30041}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I126</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{001F0020-0013-4772-9376-002400C700F3}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E90090-00EE-4E3B-B26B-00600015003C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3355,7 +3370,24 @@
           <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00E20063-0018-4CCB-809E-002A00CC00E0}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00FD0055-00CC-4B11-985F-007A001300D7}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I128</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00050081-00D9-4784-A591-0022007300E7}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3372,7 +3404,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0071008E-006B-44D6-9546-001C000A0072}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B20056-007E-449A-B728-00C800E500B4}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3389,7 +3421,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005000F5-0071-48F1-9A7B-00CB00BA0014}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0029009F-00F9-4AC0-A282-002500AB00A5}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3406,7 +3438,7 @@
           <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005A00CF-0042-4F40-8A5A-00AE008A00B7}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00860027-00DB-4C45-A9AC-00B3001E00C9}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3423,7 +3455,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003B00B9-002A-4928-B097-005D001D0050}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00560040-0089-47DC-BFEE-003000270052}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3440,7 +3472,7 @@
           <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F40030-0029-41D4-9AFA-001600880057}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001C003D-00BC-4B1E-9E3B-001F00C60014}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3457,7 +3489,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005B001A-0073-4CB3-99DD-003C00D6004A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00CD00F8-0001-4506-A7C5-0047008E000A}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3474,7 +3506,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0098003E-00F1-43F7-90AF-00D200850028}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0054004D-003A-4874-9E66-0032002600D2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3491,7 +3523,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00A900C8-00BE-4718-9675-0004000600F7}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000F009C-001A-4EAA-A737-00AF00CA002C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3508,7 +3540,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00DF00C6-00AB-4950-A644-009F0041003E}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0050004B-00AD-49D2-9EFE-005000C8007F}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3525,24 +3557,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005E00AD-00BC-401D-9FC8-0094000F008B}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I126</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00A100D4-00A9-41C2-97C0-007900BF00EF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00DC0042-00CE-4776-BEB8-00ED00040054}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3559,7 +3574,24 @@
           <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00F400F7-005D-43C5-B87F-00070092007D}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{006F006E-00AF-4305-9014-001F007500D9}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I128</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" priority="2" id="{0037003F-0055-4855-B1F9-00C600A5005F}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3575,7 +3607,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00F800B6-007A-4972-B26C-009D003E00CF}">
+          <x14:cfRule type="dataBar" priority="1" id="{00550029-0018-461C-ACFB-0084003400DC}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
tested comm & image mission completion
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -1167,7 +1167,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1222,13 +1222,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.29921259842519687</v>
+        <v>0.32283464566929132</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I123,"0")/ROWS(Table5[])</f>
-        <v>2.3622047244094488e-002</v>
+        <v>0</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1300,7 +1300,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -2045,7 +2045,9 @@
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="6"/>
+      <c r="I54" s="6">
+        <v>1</v>
+      </c>
       <c r="J54" s="9" t="s">
         <v>73</v>
       </c>
@@ -2390,7 +2392,7 @@
       <c r="I75" s="6"/>
       <c r="J75" s="9"/>
     </row>
-    <row r="76" ht="14.25">
+    <row r="76" ht="28.5">
       <c r="A76" s="11"/>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -2625,9 +2627,7 @@
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
-      <c r="I91" s="6">
-        <v>0</v>
-      </c>
+      <c r="I91" s="6"/>
       <c r="J91" s="9" t="s">
         <v>120</v>
       </c>
@@ -2644,7 +2644,7 @@
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J92" s="9"/>
     </row>
@@ -2660,7 +2660,7 @@
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J93" s="9"/>
     </row>
@@ -3183,7 +3183,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002D0065-003C-4D28-8EC3-000A00280039}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00980056-00DD-4D62-9ABD-00E5009000F0}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3200,7 +3200,7 @@
           <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00DA0000-0025-4818-A4C2-0054003E00BE}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D500C0-00F3-421D-88DB-005900BF007D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3217,7 +3217,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007100AE-00AF-48D4-A39A-004C00AB00BD}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007800AA-00C6-4EDA-B3A8-00C9001700D3}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3234,7 +3234,7 @@
           <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{009C000C-0079-4FFB-BDE8-003E00D70094}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003F00FE-00DB-4B98-9DFD-006D0003004D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3251,7 +3251,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0078003B-00FA-4C92-8184-00B700BC00C3}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{001F00EB-004F-4778-8DA1-00830046002D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3268,7 +3268,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00190060-00FB-4E7F-ABF5-000B00690071}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00C10064-0050-433F-B7D5-00CA00740014}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3285,7 +3285,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00030022-0018-490F-8EF4-00D0008200E6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0001009F-00A2-4BD7-BDCB-00070077008B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3302,7 +3302,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B2002F-0043-4571-84F5-006100BE0012}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006E0096-001B-44CE-B927-0084000C007E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3319,7 +3319,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{001300B7-0041-4538-B59C-005C00680005}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00CD0089-0028-42D5-9884-008C004300BC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3336,7 +3336,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{000800EF-002B-44DD-AA3F-002400DE0075}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0096007A-0046-4643-8BF1-00F000020078}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3353,7 +3353,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E90090-00EE-4E3B-B26B-00600015003C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007500B0-0089-4590-816F-0086008300CB}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3370,7 +3370,7 @@
           <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00FD0055-00CC-4B11-985F-007A001300D7}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00C90035-0019-47DA-B175-00A400D10030}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3387,7 +3387,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00050081-00D9-4784-A591-0022007300E7}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00290057-00B0-4F63-BB6B-00A9004F0006}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3404,7 +3404,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B20056-007E-449A-B728-00C800E500B4}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00DA002B-001E-4411-9233-007500310011}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3421,7 +3421,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0029009F-00F9-4AC0-A282-002500AB00A5}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005A0005-00C5-4DED-B89B-00EB000100FA}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3438,7 +3438,7 @@
           <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00860027-00DB-4C45-A9AC-00B3001E00C9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D90001-001D-4FA4-8DEC-0076001B00CA}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3455,7 +3455,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00560040-0089-47DC-BFEE-003000270052}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BB007E-0031-4109-AA60-008200310073}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3472,7 +3472,7 @@
           <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001C003D-00BC-4B1E-9E3B-001F00C60014}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0017009E-0020-4991-8BA4-00FE00C90048}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3489,7 +3489,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00CD00F8-0001-4506-A7C5-0047008E000A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003B00C7-009D-4AD6-915A-00E100BA007F}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3506,7 +3506,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0054004D-003A-4874-9E66-0032002600D2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00250025-006F-4B15-8999-00A200B200B6}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3523,7 +3523,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000F009C-001A-4EAA-A737-00AF00CA002C}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000B0026-00F1-4FAF-8D6A-00BE00B3006C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3540,7 +3540,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0050004B-00AD-49D2-9EFE-005000C8007F}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D400FC-0093-47AC-AD4C-003600910083}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3557,7 +3557,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00DC0042-00CE-4776-BEB8-00ED00040054}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{009D001E-0058-4633-ADB3-000E007600C4}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3574,7 +3574,7 @@
           <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{006F006E-00AF-4305-9014-001F007500D9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003600C7-0056-4D13-9380-00CF005E005B}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3591,7 +3591,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{0037003F-0055-4855-B1F9-00C600A5005F}">
+          <x14:cfRule type="dataBar" priority="2" id="{00A20075-0039-473D-8092-0005009B0057}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3607,7 +3607,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00550029-0018-461C-ACFB-0084003400DC}">
+          <x14:cfRule type="dataBar" priority="1" id="{009A006C-00C1-4348-A035-00C20052002B}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
added skeleton for mission list UI
</commit_message>
<xml_diff>
--- a/Project Work Breakdown Structure.xlsx
+++ b/Project Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>Status</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t xml:space="preserve">show points when selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show reward</t>
   </si>
   <si>
     <t>Time-scaling</t>
@@ -657,7 +660,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J128" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J129" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1167,7 +1170,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1222,13 +1225,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.32283464566929132</v>
+        <v>0.3203125</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I123,"0")/ROWS(Table5[])</f>
-        <v>0</v>
+        <f>COUNTIF(I2:I124,"0")/ROWS(Table5[])</f>
+        <v>2.34375e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1265,7 +1268,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -2913,7 +2916,9 @@
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="6"/>
+      <c r="I111" s="6">
+        <v>0</v>
+      </c>
       <c r="J111" s="9"/>
     </row>
     <row r="112" ht="14.25">
@@ -2927,7 +2932,9 @@
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
-      <c r="I112" s="6"/>
+      <c r="I112" s="6">
+        <v>0</v>
+      </c>
       <c r="J112" s="9"/>
     </row>
     <row r="113" ht="14.25">
@@ -2941,7 +2948,9 @@
       </c>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="6"/>
+      <c r="I113" s="6">
+        <v>0</v>
+      </c>
       <c r="J113" s="9"/>
     </row>
     <row r="114" ht="14.25">
@@ -2976,26 +2985,24 @@
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
-      <c r="I116" s="6">
-        <v>1</v>
-      </c>
+      <c r="I116" s="6"/>
       <c r="J116" s="9"/>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-      <c r="E117" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D117" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E117" s="4"/>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
@@ -3010,7 +3017,7 @@
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
-        <v>132</v>
+        <v>7</v>
       </c>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
@@ -3023,24 +3030,26 @@
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
-      <c r="C119" s="4" t="s">
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
-      <c r="I119" s="6"/>
+      <c r="I119" s="6">
+        <v>1</v>
+      </c>
       <c r="J119" s="9"/>
     </row>
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4" t="s">
+      <c r="C120" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="D120" s="4"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
@@ -3081,7 +3090,7 @@
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
@@ -3092,11 +3101,11 @@
     </row>
     <row r="124" ht="14.25">
       <c r="A124" s="4"/>
-      <c r="B124" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="B124" s="4"/>
       <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
+      <c r="D124" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
       <c r="G124" s="4"/>
@@ -3106,25 +3115,23 @@
     </row>
     <row r="125" ht="14.25">
       <c r="A125" s="4"/>
-      <c r="B125" s="4"/>
-      <c r="C125" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="B125" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C125" s="4"/>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="6"/>
-      <c r="J125" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="J125" s="9"/>
     </row>
     <row r="126" ht="14.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -3133,38 +3140,53 @@
       <c r="H126" s="4"/>
       <c r="I126" s="6"/>
       <c r="J126" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="127" ht="14.25">
       <c r="A127" s="4"/>
-      <c r="B127" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
-      <c r="H127" s="15"/>
+      <c r="H127" s="4"/>
       <c r="I127" s="6"/>
-      <c r="J127" s="16"/>
+      <c r="J127" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="128" ht="14.25">
-      <c r="C128" t="s">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="15"/>
       <c r="I128" s="6"/>
-      <c r="J128" t="s">
+      <c r="J128" s="16"/>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="C129" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="129" ht="14.25">
-      <c r="C129" s="17"/>
-      <c r="I129" s="4"/>
-      <c r="J129" s="17"/>
-    </row>
-    <row r="130" ht="14.25"/>
+      <c r="I129" s="6"/>
+      <c r="J129" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="130" ht="14.25">
+      <c r="C130" s="17"/>
+      <c r="I130" s="4"/>
+      <c r="J130" s="17"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
@@ -3183,7 +3205,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00980056-00DD-4D62-9ABD-00E5009000F0}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F700BD-004D-4F8A-AB45-0012000400E3}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3197,10 +3219,27 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
+          <xm:sqref>I3:I111 I112:I124 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D500C0-00F3-421D-88DB-005900BF007D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00CA0013-0027-4E53-917D-00C800E8009A}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F30013-00BF-48C3-B612-001100D20021}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3217,24 +3256,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007800AA-00C6-4EDA-B3A8-00C9001700D3}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I124</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003F00FE-00DB-4B98-9DFD-006D0003004D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00180005-0027-49AA-B4EE-00C900A200AC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3251,7 +3273,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{001F00EB-004F-4778-8DA1-00830046002D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00460067-00B6-4B6A-8A16-00C3003E00C5}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3268,7 +3290,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C10064-0050-433F-B7D5-00CA00740014}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006C0066-0088-487B-AC3B-0045000E00C9}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3285,7 +3307,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0001009F-00A2-4BD7-BDCB-00070077008B}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00DD0069-00F9-4BE8-B72C-0089007E0068}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3302,7 +3324,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{006E0096-001B-44CE-B927-0084000C007E}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D20086-002E-41D0-A662-003E00800028}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3319,7 +3341,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00CD0089-0028-42D5-9884-008C004300BC}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E6000B-008D-47E5-9F73-0005000800E2}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3336,7 +3358,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0096007A-0046-4643-8BF1-00F000020078}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{009800F6-003F-4DF1-8C9F-00F5008E0044}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3353,24 +3375,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007500B0-0089-4590-816F-0086008300CB}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I127</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C90035-0019-47DA-B175-00A400D10030}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00CD007D-00B5-464C-8747-0018008F004D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3387,7 +3392,24 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00290057-00B0-4F63-BB6B-00A9004F0006}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004B0088-0020-4667-9271-00EB000B00D4}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I129</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003F0031-00F7-4745-A544-00E100080002}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3404,7 +3426,58 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00DA002B-001E-4411-9233-007500310011}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B7004B-0075-45FC-8592-00E1000F00D3}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{002900D8-0019-4438-B24A-00C300AA009A}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I3:I111 I112:I124 I46:I49</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00EB0091-0024-48B9-9E01-00D700EC007A}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B90062-001E-4FD0-B972-005E00E900ED}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3421,58 +3494,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005A0005-00C5-4DED-B89B-00EB000100FA}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I3:I111 I112:I123 I46:I49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D90001-001D-4FA4-8DEC-0076001B00CA}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BB007E-0031-4109-AA60-008200310073}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I124</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0017009E-0020-4991-8BA4-00FE00C90048}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003200EB-0052-4BE5-8DFA-000F00390040}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3489,7 +3511,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003B00C7-009D-4AD6-915A-00E100BA007F}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005A0001-004D-45F4-A81C-009400790015}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3506,7 +3528,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00250025-006F-4B15-8999-00A200B200B6}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001A002B-0063-4E0C-91FB-000A00CB00E0}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3523,7 +3545,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000B0026-00F1-4FAF-8D6A-00BE00B3006C}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BC0025-002A-4BCF-9DE2-00850051006A}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3540,7 +3562,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D400FC-0093-47AC-AD4C-003600910083}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{006F0060-00FD-4EF5-80C0-008900B50052}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3557,24 +3579,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009D001E-0058-4633-ADB3-000E007600C4}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I127</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003600C7-0056-4D13-9380-00CF005E005B}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90080-007A-4FC8-BCA6-009200A40087}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3591,7 +3596,24 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00A20075-0039-473D-8092-0005009B0057}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004000DD-0005-4FA9-9B47-008D004E00CF}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I129</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" priority="2" id="{00B00003-0043-4989-B880-005D00E90043}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3607,7 +3629,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{009A006C-00C1-4348-A035-00C20052002B}">
+          <x14:cfRule type="dataBar" priority="1" id="{00D80032-009F-4271-9CCD-0057002B00D0}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>